<commit_message>
get rid of title bar
</commit_message>
<xml_diff>
--- a/model/Squoids_data/Squoids floor builder 20180107.xlsx
+++ b/model/Squoids_data/Squoids floor builder 20180107.xlsx
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12393" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12413" uniqueCount="291">
   <si>
     <t>width</t>
   </si>
@@ -2049,6 +2049,18 @@
   <si>
     <t>t</t>
   </si>
+  <si>
+    <t>*    *        *    *</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">pT   p              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">p    p              </t>
+  </si>
 </sst>
 </file>
 
@@ -2275,6 +2287,20 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="151">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2699,20 +2725,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
         </patternFill>
       </fill>
     </dxf>
@@ -51671,7 +51683,7 @@
   <dimension ref="A1:AB30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="AA20" sqref="AA1:AA20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -51729,16 +51741,16 @@
         <v>61</v>
       </c>
       <c r="P1" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="Q1" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="R1" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="S1" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="T1" s="12" t="s">
         <v>61</v>
@@ -51754,11 +51766,11 @@
       </c>
       <c r="AA1" t="str">
         <f>CONCATENATE(A1,B1,C1,D1,E1,F1,G1,H1,I1,J1,K1,L1,M1,N1,O1,P1,Q1,R1,S1,T1,U1,V1,W1,X1,Y1)</f>
-        <v>******        *    *</v>
+        <v>******        ******</v>
       </c>
       <c r="AB1" t="str">
         <f>"'"&amp;AA1&amp;"',"</f>
-        <v>'******        *    *',</v>
+        <v>'******        ******',</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
@@ -51805,7 +51817,7 @@
         <v>6</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="P2" s="12" t="s">
         <v>6</v>
@@ -51820,7 +51832,7 @@
         <v>6</v>
       </c>
       <c r="T2" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="U2" s="6"/>
       <c r="V2" s="6"/>
@@ -51833,11 +51845,11 @@
       </c>
       <c r="AA2" t="str">
         <f t="shared" ref="AA2:AA25" si="0">CONCATENATE(A2,B2,C2,D2,E2,F2,G2,H2,I2,J2,K2,L2,M2,N2,O2,P2,Q2,R2,S2,T2,U2,V2,W2,X2,Y2)</f>
-        <v xml:space="preserve">*    *              </v>
+        <v>*    *        *    *</v>
       </c>
       <c r="AB2" t="str">
         <f t="shared" ref="AB2:AB20" si="1">"'"&amp;AA2&amp;"',"</f>
-        <v>'*    *              ',</v>
+        <v>'*    *        *    *',</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
@@ -51884,7 +51896,7 @@
         <v>6</v>
       </c>
       <c r="O3" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="P3" s="12" t="s">
         <v>6</v>
@@ -51899,7 +51911,7 @@
         <v>6</v>
       </c>
       <c r="T3" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="U3" s="6"/>
       <c r="V3" s="6"/>
@@ -51912,11 +51924,11 @@
       </c>
       <c r="AA3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">*    *              </v>
+        <v>*    *        *    *</v>
       </c>
       <c r="AB3" t="str">
         <f t="shared" si="1"/>
-        <v>'*    *              ',</v>
+        <v>'*    *        *    *',</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
@@ -51963,7 +51975,7 @@
         <v>6</v>
       </c>
       <c r="O4" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="P4" s="12" t="s">
         <v>6</v>
@@ -51978,7 +51990,7 @@
         <v>6</v>
       </c>
       <c r="T4" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="U4" s="6"/>
       <c r="V4" s="6"/>
@@ -51991,11 +52003,11 @@
       </c>
       <c r="AA4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">*    *              </v>
+        <v>*    *        *    *</v>
       </c>
       <c r="AB4" t="str">
         <f t="shared" si="1"/>
-        <v>'*    *              ',</v>
+        <v>'*    *        *    *',</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
@@ -52042,7 +52054,7 @@
         <v>6</v>
       </c>
       <c r="O5" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="P5" s="12" t="s">
         <v>6</v>
@@ -52057,7 +52069,7 @@
         <v>6</v>
       </c>
       <c r="T5" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="U5" s="6"/>
       <c r="V5" s="6"/>
@@ -52070,11 +52082,11 @@
       </c>
       <c r="AA5" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">*    *              </v>
+        <v>*    *        *    *</v>
       </c>
       <c r="AB5" t="str">
         <f t="shared" si="1"/>
-        <v>'*    *              ',</v>
+        <v>'*    *        *    *',</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
@@ -52124,16 +52136,16 @@
         <v>61</v>
       </c>
       <c r="P6" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="Q6" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="R6" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="S6" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="T6" s="12" t="s">
         <v>61</v>
@@ -52149,11 +52161,11 @@
       </c>
       <c r="AA6" t="str">
         <f t="shared" si="0"/>
-        <v>******        *    *</v>
+        <v>******        ******</v>
       </c>
       <c r="AB6" t="str">
         <f t="shared" si="1"/>
-        <v>'******        *    *',</v>
+        <v>'******        ******',</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
@@ -53505,12 +53517,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="45" priority="2">
+    <cfRule type="expression" dxfId="47" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="44" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -53524,7 +53536,7 @@
   <dimension ref="A1:AB30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA20" sqref="AA1:AA20"/>
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -55378,22 +55390,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:T6">
-    <cfRule type="expression" dxfId="43" priority="4">
+    <cfRule type="expression" dxfId="45" priority="4">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:T6">
-    <cfRule type="cellIs" dxfId="41" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="3" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:F6">
-    <cfRule type="expression" dxfId="39" priority="2">
+    <cfRule type="expression" dxfId="41" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:F6">
-    <cfRule type="cellIs" dxfId="37" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -55407,7 +55419,7 @@
   <dimension ref="A1:AB30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:G14"/>
+      <selection activeCell="AA20" sqref="AA1:AA20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -55488,9 +55500,8 @@
         <f>ROW()</f>
         <v>1</v>
       </c>
-      <c r="AA1" t="str">
-        <f>CONCATENATE(A1,B1,C1,D1,E1,F1,G1,H1,I1,J1,K1,L1,M1,N1,O1,P1,Q1,R1,S1,T1,U1,V1,W1,X1,Y1)</f>
-        <v>*    *        *    *</v>
+      <c r="AA1" t="s">
+        <v>287</v>
       </c>
       <c r="AB1" t="str">
         <f>"'"&amp;AA1&amp;"',"</f>
@@ -55567,12 +55578,11 @@
         <f>ROW()</f>
         <v>2</v>
       </c>
-      <c r="AA2" t="str">
-        <f t="shared" ref="AA2:AA25" si="0">CONCATENATE(A2,B2,C2,D2,E2,F2,G2,H2,I2,J2,K2,L2,M2,N2,O2,P2,Q2,R2,S2,T2,U2,V2,W2,X2,Y2)</f>
-        <v xml:space="preserve">                    </v>
+      <c r="AA2" t="s">
+        <v>288</v>
       </c>
       <c r="AB2" t="str">
-        <f t="shared" ref="AB2:AB20" si="1">"'"&amp;AA2&amp;"',"</f>
+        <f t="shared" ref="AB2:AB20" si="0">"'"&amp;AA2&amp;"',"</f>
         <v>'                    ',</v>
       </c>
     </row>
@@ -55646,12 +55656,11 @@
         <f>ROW()</f>
         <v>3</v>
       </c>
-      <c r="AA3" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">                    </v>
+      <c r="AA3" t="s">
+        <v>288</v>
       </c>
       <c r="AB3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>'                    ',</v>
       </c>
     </row>
@@ -55725,12 +55734,11 @@
         <f>ROW()</f>
         <v>4</v>
       </c>
-      <c r="AA4" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">                    </v>
+      <c r="AA4" t="s">
+        <v>288</v>
       </c>
       <c r="AB4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>'                    ',</v>
       </c>
     </row>
@@ -55804,12 +55812,11 @@
         <f>ROW()</f>
         <v>5</v>
       </c>
-      <c r="AA5" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">                    </v>
+      <c r="AA5" t="s">
+        <v>288</v>
       </c>
       <c r="AB5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>'                    ',</v>
       </c>
     </row>
@@ -55883,12 +55890,11 @@
         <f>ROW()</f>
         <v>6</v>
       </c>
-      <c r="AA6" t="str">
-        <f t="shared" si="0"/>
-        <v>*    *        *    *</v>
+      <c r="AA6" t="s">
+        <v>287</v>
       </c>
       <c r="AB6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>'*    *        *    *',</v>
       </c>
     </row>
@@ -55962,12 +55968,11 @@
         <f>ROW()</f>
         <v>7</v>
       </c>
-      <c r="AA7" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">                    </v>
+      <c r="AA7" t="s">
+        <v>288</v>
       </c>
       <c r="AB7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>'                    ',</v>
       </c>
     </row>
@@ -56041,12 +56046,11 @@
         <f>ROW()</f>
         <v>8</v>
       </c>
-      <c r="AA8" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">                    </v>
+      <c r="AA8" t="s">
+        <v>288</v>
       </c>
       <c r="AB8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>'                    ',</v>
       </c>
     </row>
@@ -56120,12 +56124,11 @@
         <f>ROW()</f>
         <v>9</v>
       </c>
-      <c r="AA9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">                    </v>
+      <c r="AA9" t="s">
+        <v>288</v>
       </c>
       <c r="AB9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>'                    ',</v>
       </c>
     </row>
@@ -56199,12 +56202,11 @@
         <f>ROW()</f>
         <v>10</v>
       </c>
-      <c r="AA10" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">                    </v>
+      <c r="AA10" t="s">
+        <v>288</v>
       </c>
       <c r="AB10" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>'                    ',</v>
       </c>
     </row>
@@ -56278,12 +56280,11 @@
         <f>ROW()</f>
         <v>11</v>
       </c>
-      <c r="AA11" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">                    </v>
+      <c r="AA11" t="s">
+        <v>288</v>
       </c>
       <c r="AB11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>'                    ',</v>
       </c>
     </row>
@@ -56357,12 +56358,11 @@
         <f>ROW()</f>
         <v>12</v>
       </c>
-      <c r="AA12" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">                    </v>
+      <c r="AA12" t="s">
+        <v>288</v>
       </c>
       <c r="AB12" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>'                    ',</v>
       </c>
     </row>
@@ -56436,12 +56436,11 @@
         <f>ROW()</f>
         <v>13</v>
       </c>
-      <c r="AA13" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">                    </v>
+      <c r="AA13" t="s">
+        <v>288</v>
       </c>
       <c r="AB13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>'                    ',</v>
       </c>
     </row>
@@ -56515,12 +56514,11 @@
         <f>ROW()</f>
         <v>14</v>
       </c>
-      <c r="AA14" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">                    </v>
+      <c r="AA14" t="s">
+        <v>288</v>
       </c>
       <c r="AB14" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>'                    ',</v>
       </c>
     </row>
@@ -56594,12 +56592,11 @@
         <f>ROW()</f>
         <v>15</v>
       </c>
-      <c r="AA15" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">pT   p              </v>
+      <c r="AA15" t="s">
+        <v>289</v>
       </c>
       <c r="AB15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>'pT   p              ',</v>
       </c>
     </row>
@@ -56673,12 +56670,11 @@
         <f>ROW()</f>
         <v>16</v>
       </c>
-      <c r="AA16" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">                    </v>
+      <c r="AA16" t="s">
+        <v>288</v>
       </c>
       <c r="AB16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>'                    ',</v>
       </c>
     </row>
@@ -56752,12 +56748,11 @@
         <f>ROW()</f>
         <v>17</v>
       </c>
-      <c r="AA17" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">                    </v>
+      <c r="AA17" t="s">
+        <v>288</v>
       </c>
       <c r="AB17" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>'                    ',</v>
       </c>
     </row>
@@ -56831,12 +56826,11 @@
         <f>ROW()</f>
         <v>18</v>
       </c>
-      <c r="AA18" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">                    </v>
+      <c r="AA18" t="s">
+        <v>288</v>
       </c>
       <c r="AB18" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>'                    ',</v>
       </c>
     </row>
@@ -56910,12 +56904,11 @@
         <f>ROW()</f>
         <v>19</v>
       </c>
-      <c r="AA19" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">                    </v>
+      <c r="AA19" t="s">
+        <v>288</v>
       </c>
       <c r="AB19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>'                    ',</v>
       </c>
     </row>
@@ -56989,12 +56982,11 @@
         <f>ROW()</f>
         <v>20</v>
       </c>
-      <c r="AA20" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">p    p              </v>
+      <c r="AA20" t="s">
+        <v>290</v>
       </c>
       <c r="AB20" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>'p    p              ',</v>
       </c>
     </row>
@@ -57085,7 +57077,7 @@
       <c r="X21" s="6"/>
       <c r="Y21" s="7"/>
       <c r="AA21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="AA2:AA25" si="1">CONCATENATE(A21,B21,C21,D21,E21,F21,G21,H21,I21,J21,K21,L21,M21,N21,O21,P21,Q21,R21,S21,T21,U21,V21,W21,X21,Y21)</f>
         <v>1234567891011121314151617181920</v>
       </c>
     </row>
@@ -57116,7 +57108,7 @@
       <c r="X22" s="6"/>
       <c r="Y22" s="7"/>
       <c r="AA22" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -57147,7 +57139,7 @@
       <c r="X23" s="6"/>
       <c r="Y23" s="7"/>
       <c r="AA23" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -57178,7 +57170,7 @@
       <c r="X24" s="6"/>
       <c r="Y24" s="7"/>
       <c r="AA24" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -57209,7 +57201,7 @@
       <c r="X25" s="10"/>
       <c r="Y25" s="11"/>
       <c r="AA25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -57256,17 +57248,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:E5">
-    <cfRule type="cellIs" dxfId="61" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="3" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:T6">
-    <cfRule type="expression" dxfId="29" priority="2">
+    <cfRule type="expression" dxfId="31" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:T6">
-    <cfRule type="cellIs" dxfId="27" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -59144,32 +59136,32 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6">
-    <cfRule type="expression" dxfId="19" priority="6">
+    <cfRule type="expression" dxfId="21" priority="6">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6">
-    <cfRule type="cellIs" dxfId="17" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="5" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1">
-    <cfRule type="expression" dxfId="15" priority="4">
+    <cfRule type="expression" dxfId="17" priority="4">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1">
-    <cfRule type="cellIs" dxfId="13" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="3" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6">
-    <cfRule type="expression" dxfId="11" priority="2">
+    <cfRule type="expression" dxfId="13" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6">
-    <cfRule type="cellIs" dxfId="9" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Citadel improvements + weapon graphics
</commit_message>
<xml_diff>
--- a/model/Squoids_data/Squoids floor builder 20180107.xlsx
+++ b/model/Squoids_data/Squoids floor builder 20180107.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7770" windowHeight="540" tabRatio="904" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7770" windowHeight="540" tabRatio="904" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Reverser" sheetId="33" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12413" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12396" uniqueCount="287">
   <si>
     <t>width</t>
   </si>
@@ -2049,18 +2049,6 @@
   <si>
     <t>t</t>
   </si>
-  <si>
-    <t>*    *        *    *</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">pT   p              </t>
-  </si>
-  <si>
-    <t xml:space="preserve">p    p              </t>
-  </si>
 </sst>
 </file>
 
@@ -2286,427 +2274,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="151">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="125">
     <dxf>
       <fill>
         <patternFill>
@@ -3347,6 +2915,244 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -6127,12 +5933,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y26">
-    <cfRule type="expression" dxfId="150" priority="2">
+    <cfRule type="expression" dxfId="124" priority="2">
       <formula>AND(COLUMN()&lt;=$B$27,ROW()&lt;=$B$28)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z26">
-    <cfRule type="cellIs" dxfId="149" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7980,25 +7786,25 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y5 A6:D8 H6:Y8 A9:Y25">
-    <cfRule type="expression" dxfId="146" priority="5">
+    <cfRule type="expression" dxfId="86" priority="5">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z5 A6:D8 H6:Z8 A9:Z25">
-    <cfRule type="cellIs" dxfId="145" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="4" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA2:AA20">
-    <cfRule type="uniqueValues" dxfId="144" priority="3"/>
+    <cfRule type="uniqueValues" dxfId="84" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6:G8">
-    <cfRule type="expression" dxfId="143" priority="2">
+    <cfRule type="expression" dxfId="83" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6:G8">
-    <cfRule type="cellIs" dxfId="142" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9846,12 +9652,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="141" priority="2">
+    <cfRule type="expression" dxfId="81" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="140" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11699,12 +11505,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="139" priority="2">
+    <cfRule type="expression" dxfId="79" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="138" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13552,12 +13358,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="137" priority="2">
+    <cfRule type="expression" dxfId="77" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="136" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15405,12 +15211,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="135" priority="2">
+    <cfRule type="expression" dxfId="75" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="134" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17261,12 +17067,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="133" priority="2">
+    <cfRule type="expression" dxfId="73" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="132" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18994,22 +18800,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A21:Y25 U1:Y20">
-    <cfRule type="expression" dxfId="131" priority="4">
+    <cfRule type="expression" dxfId="71" priority="4">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:Z25 U1:Z20">
-    <cfRule type="cellIs" dxfId="130" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="3" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:T20">
-    <cfRule type="expression" dxfId="129" priority="2">
+    <cfRule type="expression" dxfId="69" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:T20">
-    <cfRule type="cellIs" dxfId="128" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20735,22 +20541,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A21:Y25 U1:Y20 A19">
-    <cfRule type="expression" dxfId="127" priority="4">
+    <cfRule type="expression" dxfId="67" priority="4">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:Z25 U1:Z20 A19">
-    <cfRule type="cellIs" dxfId="126" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="3" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20 A1:T2 A3:A18 B3:T20">
-    <cfRule type="expression" dxfId="125" priority="2">
+    <cfRule type="expression" dxfId="65" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20 A1:T2 A3:A18 B3:T20">
-    <cfRule type="cellIs" dxfId="124" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22482,22 +22288,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A21:Y25 U1:Y20">
-    <cfRule type="expression" dxfId="123" priority="4">
+    <cfRule type="expression" dxfId="63" priority="4">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:Z25 U1:Z20">
-    <cfRule type="cellIs" dxfId="122" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="3" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:T20">
-    <cfRule type="expression" dxfId="121" priority="2">
+    <cfRule type="expression" dxfId="61" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:T20">
-    <cfRule type="cellIs" dxfId="120" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -24225,22 +24031,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A21:Y25 U1:Y20">
-    <cfRule type="expression" dxfId="119" priority="4">
+    <cfRule type="expression" dxfId="59" priority="4">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:Z25 U1:Z20">
-    <cfRule type="cellIs" dxfId="118" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="3" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:T20">
-    <cfRule type="expression" dxfId="117" priority="2">
+    <cfRule type="expression" dxfId="57" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:T20">
-    <cfRule type="cellIs" dxfId="116" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -26088,12 +25894,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="148" priority="2">
+    <cfRule type="expression" dxfId="122" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="147" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="121" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27821,22 +27627,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A21:Y25 U1:Y20">
-    <cfRule type="expression" dxfId="115" priority="4">
+    <cfRule type="expression" dxfId="55" priority="4">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:Z25 U1:Z20">
-    <cfRule type="cellIs" dxfId="114" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="3" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:T20">
-    <cfRule type="expression" dxfId="113" priority="2">
+    <cfRule type="expression" dxfId="53" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:T20">
-    <cfRule type="cellIs" dxfId="112" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -29564,12 +29370,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="111" priority="2">
+    <cfRule type="expression" dxfId="51" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="110" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -31297,12 +31103,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="109" priority="2">
+    <cfRule type="expression" dxfId="49" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="108" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -33030,12 +32836,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="107" priority="2">
+    <cfRule type="expression" dxfId="47" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="106" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -34763,22 +34569,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A21:Y25 U1:Y20">
-    <cfRule type="expression" dxfId="105" priority="4">
+    <cfRule type="expression" dxfId="45" priority="4">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:Z25 U1:Z20">
-    <cfRule type="cellIs" dxfId="104" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="3" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:T20">
-    <cfRule type="expression" dxfId="103" priority="2">
+    <cfRule type="expression" dxfId="43" priority="2">
       <formula>AND(COLUMN()&lt;=$B$27,ROW()&lt;=$B$28)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:T20">
-    <cfRule type="cellIs" dxfId="102" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -36506,12 +36312,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="101" priority="2">
+    <cfRule type="expression" dxfId="41" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="100" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -38239,12 +38045,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="99" priority="2">
+    <cfRule type="expression" dxfId="39" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="98" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -39970,12 +39776,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="97" priority="2">
+    <cfRule type="expression" dxfId="37" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="96" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -41823,12 +41629,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="95" priority="2">
+    <cfRule type="expression" dxfId="35" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="94" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -43676,12 +43482,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="93" priority="2">
+    <cfRule type="expression" dxfId="33" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="92" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -43694,8 +43500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AA20" sqref="AA1:AA20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43762,10 +43568,10 @@
         <v>25</v>
       </c>
       <c r="S1" s="12" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="T1" s="12" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="U1" s="2"/>
       <c r="V1" s="2"/>
@@ -43778,11 +43584,11 @@
       </c>
       <c r="AA1" t="str">
         <f>CONCATENATE(A1,B1,C1,D1,E1,F1,G1,H1,I1,J1,K1,L1,M1,N1,O1,P1,Q1,R1,S1,T1,U1,V1,W1,X1,Y1)</f>
-        <v>~~~~~~~~~~~~~~~~~~~~</v>
+        <v xml:space="preserve">~~~~~~~~~~~~~~~~~~  </v>
       </c>
       <c r="AB1" t="str">
         <f>"'"&amp;AA1&amp;"',"</f>
-        <v>'~~~~~~~~~~~~~~~~~~~~',</v>
+        <v>'~~~~~~~~~~~~~~~~~~  ',</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
@@ -43790,19 +43596,19 @@
         <v>25</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="G2" s="12" t="s">
         <v>25</v>
@@ -43826,16 +43632,16 @@
         <v>25</v>
       </c>
       <c r="N2" s="12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="P2" s="12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="Q2" s="12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="R2" s="12" t="s">
         <v>25</v>
@@ -43844,7 +43650,7 @@
         <v>25</v>
       </c>
       <c r="T2" s="12" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="U2" s="6"/>
       <c r="V2" s="6"/>
@@ -43857,11 +43663,11 @@
       </c>
       <c r="AA2" t="str">
         <f t="shared" ref="AA2:AA25" si="0">CONCATENATE(A2,B2,C2,D2,E2,F2,G2,H2,I2,J2,K2,L2,M2,N2,O2,P2,Q2,R2,S2,T2,U2,V2,W2,X2,Y2)</f>
-        <v>~~~~~~~~~~~~~~~~~~~~</v>
+        <v xml:space="preserve">~lllll~~~~~~~llll~~ </v>
       </c>
       <c r="AB2" t="str">
         <f t="shared" ref="AB2:AB20" si="1">"'"&amp;AA2&amp;"',"</f>
-        <v>'~~~~~~~~~~~~~~~~~~~~',</v>
+        <v>'~lllll~~~~~~~llll~~ ',</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
@@ -43869,19 +43675,19 @@
         <v>25</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="G3" s="12" t="s">
         <v>25</v>
@@ -43905,16 +43711,16 @@
         <v>25</v>
       </c>
       <c r="N3" s="12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="O3" s="12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="P3" s="12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="Q3" s="12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="R3" s="12" t="s">
         <v>25</v>
@@ -43923,7 +43729,7 @@
         <v>25</v>
       </c>
       <c r="T3" s="12" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="U3" s="6"/>
       <c r="V3" s="6"/>
@@ -43936,11 +43742,11 @@
       </c>
       <c r="AA3" t="str">
         <f t="shared" si="0"/>
-        <v>~~~~~~~~~~~~~~~~~~~~</v>
+        <v xml:space="preserve">~lllll~~~~~~~llll~~ </v>
       </c>
       <c r="AB3" t="str">
         <f t="shared" si="1"/>
-        <v>'~~~~~~~~~~~~~~~~~~~~',</v>
+        <v>'~lllll~~~~~~~llll~~ ',</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
@@ -43948,19 +43754,19 @@
         <v>25</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="G4" s="12" t="s">
         <v>25</v>
@@ -43984,16 +43790,16 @@
         <v>25</v>
       </c>
       <c r="N4" s="12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="O4" s="12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="P4" s="12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="Q4" s="12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="R4" s="12" t="s">
         <v>25</v>
@@ -44015,11 +43821,11 @@
       </c>
       <c r="AA4" t="str">
         <f t="shared" si="0"/>
-        <v>~~~~~~~~~~~~~~~~~~~~</v>
+        <v>~lllll~~~~~~~llll~~~</v>
       </c>
       <c r="AB4" t="str">
         <f t="shared" si="1"/>
-        <v>'~~~~~~~~~~~~~~~~~~~~',</v>
+        <v>'~lllll~~~~~~~llll~~~',</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
@@ -44027,19 +43833,19 @@
         <v>25</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="G5" s="12" t="s">
         <v>25</v>
@@ -44063,16 +43869,16 @@
         <v>25</v>
       </c>
       <c r="N5" s="12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="O5" s="12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="P5" s="12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="Q5" s="12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="R5" s="12" t="s">
         <v>25</v>
@@ -44094,11 +43900,11 @@
       </c>
       <c r="AA5" t="str">
         <f t="shared" si="0"/>
-        <v>~~~~~~~~~~~~~~~~~~~~</v>
+        <v>~lllll~~~~~~~llll~~~</v>
       </c>
       <c r="AB5" t="str">
         <f t="shared" si="1"/>
-        <v>'~~~~~~~~~~~~~~~~~~~~',</v>
+        <v>'~lllll~~~~~~~llll~~~',</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
@@ -44106,19 +43912,19 @@
         <v>25</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="G6" s="12" t="s">
         <v>25</v>
@@ -44142,16 +43948,16 @@
         <v>25</v>
       </c>
       <c r="N6" s="12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="O6" s="12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="P6" s="12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="Q6" s="12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="R6" s="12" t="s">
         <v>25</v>
@@ -44173,11 +43979,11 @@
       </c>
       <c r="AA6" t="str">
         <f t="shared" si="0"/>
-        <v>~~~~~~~~~~~~~~~~~~~~</v>
+        <v>~lllll~~~~~~~llll~~~</v>
       </c>
       <c r="AB6" t="str">
         <f t="shared" si="1"/>
-        <v>'~~~~~~~~~~~~~~~~~~~~',</v>
+        <v>'~lllll~~~~~~~llll~~~',</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
@@ -45108,7 +44914,7 @@
         <v>25</v>
       </c>
       <c r="T18" s="12" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="U18" s="6"/>
       <c r="V18" s="6"/>
@@ -45121,19 +44927,19 @@
       </c>
       <c r="AA18" t="str">
         <f t="shared" si="0"/>
-        <v>~~~~~~~~~~~~~~~~~~~~</v>
+        <v xml:space="preserve">~~~~~~~~~~~~~~~~~~~ </v>
       </c>
       <c r="AB18" t="str">
         <f t="shared" si="1"/>
-        <v>'~~~~~~~~~~~~~~~~~~~~',</v>
+        <v>'~~~~~~~~~~~~~~~~~~~ ',</v>
       </c>
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="C19" s="12" t="s">
         <v>25</v>
@@ -45187,7 +44993,7 @@
         <v>25</v>
       </c>
       <c r="T19" s="12" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="U19" s="6"/>
       <c r="V19" s="6"/>
@@ -45200,22 +45006,22 @@
       </c>
       <c r="AA19" t="str">
         <f t="shared" si="0"/>
-        <v>~~~~~~~~~~~~~~~~~~~~</v>
+        <v xml:space="preserve">  ~~~~~~~~~~~~~~~~~ </v>
       </c>
       <c r="AB19" t="str">
         <f t="shared" si="1"/>
-        <v>'~~~~~~~~~~~~~~~~~~~~',</v>
+        <v>'  ~~~~~~~~~~~~~~~~~ ',</v>
       </c>
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="D20" s="12" t="s">
         <v>25</v>
@@ -45260,13 +45066,13 @@
         <v>25</v>
       </c>
       <c r="R20" s="12" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="S20" s="12" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="T20" s="12" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="U20" s="6"/>
       <c r="V20" s="6"/>
@@ -45279,11 +45085,11 @@
       </c>
       <c r="AA20" t="str">
         <f t="shared" si="0"/>
-        <v>~~~~~~~~~~~~~~~~~~~~</v>
+        <v xml:space="preserve">   ~~~~~~~~~~~~~~   </v>
       </c>
       <c r="AB20" t="str">
         <f t="shared" si="1"/>
-        <v>'~~~~~~~~~~~~~~~~~~~~',</v>
+        <v>'   ~~~~~~~~~~~~~~   ',</v>
       </c>
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.25">
@@ -45529,12 +45335,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="75" priority="2">
+    <cfRule type="expression" dxfId="120" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="74" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -47382,12 +47188,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="91" priority="2">
+    <cfRule type="expression" dxfId="31" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="90" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -49235,12 +49041,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="89" priority="2">
+    <cfRule type="expression" dxfId="29" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="88" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -51654,22 +51460,22 @@
     <sortCondition ref="B2:B67"/>
   </sortState>
   <conditionalFormatting sqref="D1:D31 D33:D1048576">
-    <cfRule type="cellIs" dxfId="87" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="4" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K31 K33:K77">
-    <cfRule type="cellIs" dxfId="86" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="3" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32">
-    <cfRule type="cellIs" dxfId="85" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="2" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32">
-    <cfRule type="cellIs" dxfId="84" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -51696,7 +51502,7 @@
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>61</v>
+        <v>264</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>61</v>
@@ -51714,7 +51520,7 @@
         <v>61</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>6</v>
+        <v>264</v>
       </c>
       <c r="H1" s="12" t="s">
         <v>6</v>
@@ -51732,10 +51538,10 @@
         <v>6</v>
       </c>
       <c r="M1" s="12" t="s">
-        <v>6</v>
+        <v>264</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="O1" s="12" t="s">
         <v>61</v>
@@ -51747,13 +51553,13 @@
         <v>61</v>
       </c>
       <c r="R1" s="12" t="s">
-        <v>61</v>
+        <v>264</v>
       </c>
       <c r="S1" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="T1" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="U1" s="2"/>
       <c r="V1" s="2"/>
@@ -51766,11 +51572,11 @@
       </c>
       <c r="AA1" t="str">
         <f>CONCATENATE(A1,B1,C1,D1,E1,F1,G1,H1,I1,J1,K1,L1,M1,N1,O1,P1,Q1,R1,S1,T1,U1,V1,W1,X1,Y1)</f>
-        <v>******        ******</v>
+        <v xml:space="preserve">H*****H     H****H  </v>
       </c>
       <c r="AB1" t="str">
         <f>"'"&amp;AA1&amp;"',"</f>
-        <v>'******        ******',</v>
+        <v>'H*****H     H****H  ',</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
@@ -51790,10 +51596,10 @@
         <v>6</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="H2" s="12" t="s">
         <v>6</v>
@@ -51811,13 +51617,13 @@
         <v>6</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="N2" s="12" t="s">
         <v>6</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="P2" s="12" t="s">
         <v>6</v>
@@ -51826,13 +51632,13 @@
         <v>6</v>
       </c>
       <c r="R2" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="S2" s="12" t="s">
         <v>6</v>
       </c>
       <c r="T2" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="U2" s="6"/>
       <c r="V2" s="6"/>
@@ -51845,11 +51651,11 @@
       </c>
       <c r="AA2" t="str">
         <f t="shared" ref="AA2:AA25" si="0">CONCATENATE(A2,B2,C2,D2,E2,F2,G2,H2,I2,J2,K2,L2,M2,N2,O2,P2,Q2,R2,S2,T2,U2,V2,W2,X2,Y2)</f>
-        <v>*    *        *    *</v>
+        <v xml:space="preserve">*     *     *    *  </v>
       </c>
       <c r="AB2" t="str">
         <f t="shared" ref="AB2:AB20" si="1">"'"&amp;AA2&amp;"',"</f>
-        <v>'*    *        *    *',</v>
+        <v>'*     *     *    *  ',</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
@@ -51869,10 +51675,10 @@
         <v>6</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="H3" s="12" t="s">
         <v>6</v>
@@ -51890,13 +51696,13 @@
         <v>6</v>
       </c>
       <c r="M3" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="N3" s="12" t="s">
         <v>6</v>
       </c>
       <c r="O3" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="P3" s="12" t="s">
         <v>6</v>
@@ -51905,13 +51711,13 @@
         <v>6</v>
       </c>
       <c r="R3" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="S3" s="12" t="s">
         <v>6</v>
       </c>
       <c r="T3" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="U3" s="6"/>
       <c r="V3" s="6"/>
@@ -51924,11 +51730,11 @@
       </c>
       <c r="AA3" t="str">
         <f t="shared" si="0"/>
-        <v>*    *        *    *</v>
+        <v xml:space="preserve">*     *     *    *  </v>
       </c>
       <c r="AB3" t="str">
         <f t="shared" si="1"/>
-        <v>'*    *        *    *',</v>
+        <v>'*     *     *    *  ',</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
@@ -51948,10 +51754,10 @@
         <v>6</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="H4" s="12" t="s">
         <v>6</v>
@@ -51969,13 +51775,13 @@
         <v>6</v>
       </c>
       <c r="M4" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="N4" s="12" t="s">
         <v>6</v>
       </c>
       <c r="O4" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="P4" s="12" t="s">
         <v>6</v>
@@ -51984,13 +51790,13 @@
         <v>6</v>
       </c>
       <c r="R4" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="S4" s="12" t="s">
         <v>6</v>
       </c>
       <c r="T4" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="U4" s="6"/>
       <c r="V4" s="6"/>
@@ -52003,11 +51809,11 @@
       </c>
       <c r="AA4" t="str">
         <f t="shared" si="0"/>
-        <v>*    *        *    *</v>
+        <v xml:space="preserve">*     *     *    *  </v>
       </c>
       <c r="AB4" t="str">
         <f t="shared" si="1"/>
-        <v>'*    *        *    *',</v>
+        <v>'*     *     *    *  ',</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
@@ -52027,10 +51833,10 @@
         <v>6</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="H5" s="12" t="s">
         <v>6</v>
@@ -52048,13 +51854,13 @@
         <v>6</v>
       </c>
       <c r="M5" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="N5" s="12" t="s">
         <v>6</v>
       </c>
       <c r="O5" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="P5" s="12" t="s">
         <v>6</v>
@@ -52063,13 +51869,13 @@
         <v>6</v>
       </c>
       <c r="R5" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="S5" s="12" t="s">
         <v>6</v>
       </c>
       <c r="T5" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="U5" s="6"/>
       <c r="V5" s="6"/>
@@ -52082,11 +51888,11 @@
       </c>
       <c r="AA5" t="str">
         <f t="shared" si="0"/>
-        <v>*    *        *    *</v>
+        <v xml:space="preserve">*     *     *    *  </v>
       </c>
       <c r="AB5" t="str">
         <f t="shared" si="1"/>
-        <v>'*    *        *    *',</v>
+        <v>'*     *     *    *  ',</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
@@ -52094,22 +51900,22 @@
         <v>61</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="H6" s="12" t="s">
         <v>6</v>
@@ -52127,28 +51933,28 @@
         <v>6</v>
       </c>
       <c r="M6" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="N6" s="12" t="s">
         <v>6</v>
       </c>
       <c r="O6" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="P6" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="Q6" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="R6" s="12" t="s">
         <v>61</v>
       </c>
       <c r="S6" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="T6" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="U6" s="6"/>
       <c r="V6" s="6"/>
@@ -52161,34 +51967,34 @@
       </c>
       <c r="AA6" t="str">
         <f t="shared" si="0"/>
-        <v>******        ******</v>
+        <v xml:space="preserve">*     *     *    *  </v>
       </c>
       <c r="AB6" t="str">
         <f t="shared" si="1"/>
-        <v>'******        ******',</v>
+        <v>'*     *     *    *  ',</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>6</v>
+        <v>264</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>6</v>
+        <v>264</v>
       </c>
       <c r="H7" s="12" t="s">
         <v>6</v>
@@ -52206,22 +52012,22 @@
         <v>6</v>
       </c>
       <c r="M7" s="12" t="s">
-        <v>6</v>
+        <v>264</v>
       </c>
       <c r="N7" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="O7" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="P7" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="Q7" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="R7" s="12" t="s">
-        <v>6</v>
+        <v>264</v>
       </c>
       <c r="S7" s="12" t="s">
         <v>6</v>
@@ -52240,11 +52046,11 @@
       </c>
       <c r="AA7" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">                    </v>
+        <v xml:space="preserve">H*****H     H****H  </v>
       </c>
       <c r="AB7" t="str">
         <f t="shared" si="1"/>
-        <v>'                    ',</v>
+        <v>'H*****H     H****H  ',</v>
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
@@ -52580,7 +52386,7 @@
         <v>6</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>6</v>
+        <v>264</v>
       </c>
       <c r="G12" s="12" t="s">
         <v>6</v>
@@ -52598,22 +52404,22 @@
         <v>6</v>
       </c>
       <c r="L12" s="12" t="s">
-        <v>6</v>
+        <v>264</v>
       </c>
       <c r="M12" s="12" t="s">
-        <v>6</v>
+        <v>285</v>
       </c>
       <c r="N12" s="12" t="s">
-        <v>6</v>
+        <v>285</v>
       </c>
       <c r="O12" s="12" t="s">
-        <v>6</v>
+        <v>285</v>
       </c>
       <c r="P12" s="12" t="s">
-        <v>6</v>
+        <v>285</v>
       </c>
       <c r="Q12" s="12" t="s">
-        <v>6</v>
+        <v>264</v>
       </c>
       <c r="R12" s="12" t="s">
         <v>6</v>
@@ -52635,11 +52441,11 @@
       </c>
       <c r="AA12" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">                    </v>
+        <v xml:space="preserve">     H     H@@@@H   </v>
       </c>
       <c r="AB12" t="str">
         <f t="shared" si="1"/>
-        <v>'                    ',</v>
+        <v>'     H     H@@@@H   ',</v>
       </c>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.25">
@@ -52677,22 +52483,22 @@
         <v>6</v>
       </c>
       <c r="L13" s="12" t="s">
-        <v>6</v>
+        <v>285</v>
       </c>
       <c r="M13" s="12" t="s">
-        <v>6</v>
+        <v>285</v>
       </c>
       <c r="N13" s="12" t="s">
-        <v>6</v>
+        <v>285</v>
       </c>
       <c r="O13" s="12" t="s">
-        <v>6</v>
+        <v>285</v>
       </c>
       <c r="P13" s="12" t="s">
-        <v>6</v>
+        <v>285</v>
       </c>
       <c r="Q13" s="12" t="s">
-        <v>6</v>
+        <v>285</v>
       </c>
       <c r="R13" s="12" t="s">
         <v>6</v>
@@ -52714,11 +52520,11 @@
       </c>
       <c r="AA13" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">                    </v>
+        <v xml:space="preserve">           @@@@@@   </v>
       </c>
       <c r="AB13" t="str">
         <f t="shared" si="1"/>
-        <v>'                    ',</v>
+        <v>'           @@@@@@   ',</v>
       </c>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.25">
@@ -52756,22 +52562,22 @@
         <v>6</v>
       </c>
       <c r="L14" s="12" t="s">
-        <v>6</v>
+        <v>285</v>
       </c>
       <c r="M14" s="12" t="s">
-        <v>6</v>
+        <v>285</v>
       </c>
       <c r="N14" s="12" t="s">
-        <v>6</v>
+        <v>285</v>
       </c>
       <c r="O14" s="12" t="s">
-        <v>6</v>
+        <v>285</v>
       </c>
       <c r="P14" s="12" t="s">
-        <v>6</v>
+        <v>285</v>
       </c>
       <c r="Q14" s="12" t="s">
-        <v>6</v>
+        <v>285</v>
       </c>
       <c r="R14" s="12" t="s">
         <v>6</v>
@@ -52793,16 +52599,16 @@
       </c>
       <c r="AA14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">                    </v>
+        <v xml:space="preserve">           @@@@@@   </v>
       </c>
       <c r="AB14" t="str">
         <f t="shared" si="1"/>
-        <v>'                    ',</v>
+        <v>'           @@@@@@   ',</v>
       </c>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="B15" s="12" t="s">
         <v>6</v>
@@ -52817,7 +52623,7 @@
         <v>6</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="G15" s="12" t="s">
         <v>6</v>
@@ -52835,31 +52641,31 @@
         <v>6</v>
       </c>
       <c r="L15" s="12" t="s">
-        <v>6</v>
+        <v>285</v>
       </c>
       <c r="M15" s="12" t="s">
-        <v>6</v>
+        <v>285</v>
       </c>
       <c r="N15" s="12" t="s">
-        <v>6</v>
+        <v>285</v>
       </c>
       <c r="O15" s="12" t="s">
-        <v>61</v>
+        <v>285</v>
       </c>
       <c r="P15" s="12" t="s">
-        <v>61</v>
+        <v>285</v>
       </c>
       <c r="Q15" s="12" t="s">
-        <v>61</v>
+        <v>285</v>
       </c>
       <c r="R15" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="S15" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="T15" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="U15" s="6"/>
       <c r="V15" s="6"/>
@@ -52872,11 +52678,11 @@
       </c>
       <c r="AA15" t="str">
         <f t="shared" si="0"/>
-        <v>*    *        ******</v>
+        <v xml:space="preserve">           @@@@@@   </v>
       </c>
       <c r="AB15" t="str">
         <f t="shared" si="1"/>
-        <v>'*    *        ******',</v>
+        <v>'           @@@@@@   ',</v>
       </c>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.25">
@@ -52914,31 +52720,31 @@
         <v>6</v>
       </c>
       <c r="L16" s="12" t="s">
-        <v>6</v>
+        <v>285</v>
       </c>
       <c r="M16" s="12" t="s">
-        <v>6</v>
+        <v>285</v>
       </c>
       <c r="N16" s="12" t="s">
-        <v>6</v>
+        <v>285</v>
       </c>
       <c r="O16" s="12" t="s">
-        <v>61</v>
+        <v>285</v>
       </c>
       <c r="P16" s="12" t="s">
-        <v>61</v>
+        <v>285</v>
       </c>
       <c r="Q16" s="12" t="s">
-        <v>61</v>
+        <v>285</v>
       </c>
       <c r="R16" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="S16" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="T16" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="U16" s="6"/>
       <c r="V16" s="6"/>
@@ -52951,16 +52757,16 @@
       </c>
       <c r="AA16" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">              ******</v>
+        <v xml:space="preserve">           @@@@@@   </v>
       </c>
       <c r="AB16" t="str">
         <f t="shared" si="1"/>
-        <v>'              ******',</v>
+        <v>'           @@@@@@   ',</v>
       </c>
     </row>
     <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>6</v>
+        <v>264</v>
       </c>
       <c r="B17" s="12" t="s">
         <v>6</v>
@@ -52975,7 +52781,7 @@
         <v>6</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>6</v>
+        <v>264</v>
       </c>
       <c r="G17" s="12" t="s">
         <v>6</v>
@@ -52993,31 +52799,31 @@
         <v>6</v>
       </c>
       <c r="L17" s="12" t="s">
-        <v>6</v>
+        <v>264</v>
       </c>
       <c r="M17" s="12" t="s">
-        <v>6</v>
+        <v>285</v>
       </c>
       <c r="N17" s="12" t="s">
-        <v>6</v>
+        <v>285</v>
       </c>
       <c r="O17" s="12" t="s">
-        <v>61</v>
+        <v>285</v>
       </c>
       <c r="P17" s="12" t="s">
-        <v>61</v>
+        <v>285</v>
       </c>
       <c r="Q17" s="12" t="s">
-        <v>61</v>
+        <v>264</v>
       </c>
       <c r="R17" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="S17" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="T17" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="U17" s="6"/>
       <c r="V17" s="6"/>
@@ -53030,11 +52836,11 @@
       </c>
       <c r="AA17" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">              ******</v>
+        <v xml:space="preserve">H    H     H@@@@H   </v>
       </c>
       <c r="AB17" t="str">
         <f t="shared" si="1"/>
-        <v>'              ******',</v>
+        <v>'H    H     H@@@@H   ',</v>
       </c>
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.25">
@@ -53081,22 +52887,22 @@
         <v>6</v>
       </c>
       <c r="O18" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="P18" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="Q18" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="R18" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="S18" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="T18" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="U18" s="6"/>
       <c r="V18" s="6"/>
@@ -53109,11 +52915,11 @@
       </c>
       <c r="AA18" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">              ******</v>
+        <v xml:space="preserve">                    </v>
       </c>
       <c r="AB18" t="str">
         <f t="shared" si="1"/>
-        <v>'              ******',</v>
+        <v>'                    ',</v>
       </c>
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.25">
@@ -53160,22 +52966,22 @@
         <v>6</v>
       </c>
       <c r="O19" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="P19" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="Q19" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="R19" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="S19" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="T19" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="U19" s="6"/>
       <c r="V19" s="6"/>
@@ -53188,16 +52994,16 @@
       </c>
       <c r="AA19" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">              ******</v>
+        <v xml:space="preserve">                    </v>
       </c>
       <c r="AB19" t="str">
         <f t="shared" si="1"/>
-        <v>'              ******',</v>
+        <v>'                    ',</v>
       </c>
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="B20" s="12" t="s">
         <v>6</v>
@@ -53212,7 +53018,7 @@
         <v>6</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="G20" s="12" t="s">
         <v>6</v>
@@ -53239,22 +53045,22 @@
         <v>6</v>
       </c>
       <c r="O20" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="P20" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="Q20" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="R20" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="S20" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="T20" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="U20" s="6"/>
       <c r="V20" s="6"/>
@@ -53267,11 +53073,11 @@
       </c>
       <c r="AA20" t="str">
         <f t="shared" si="0"/>
-        <v>*    *        ******</v>
+        <v xml:space="preserve">                    </v>
       </c>
       <c r="AB20" t="str">
         <f t="shared" si="1"/>
-        <v>'*    *        ******',</v>
+        <v>'                    ',</v>
       </c>
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.25">
@@ -53343,17 +53149,14 @@
         <f>COLUMN()</f>
         <v>17</v>
       </c>
-      <c r="R21" s="5">
-        <f>COLUMN()</f>
-        <v>18</v>
-      </c>
-      <c r="S21" s="5">
-        <f>COLUMN()</f>
-        <v>19</v>
-      </c>
-      <c r="T21" s="5">
-        <f>COLUMN()</f>
-        <v>20</v>
+      <c r="R21" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="S21" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="T21" s="12" t="s">
+        <v>6</v>
       </c>
       <c r="U21" s="6"/>
       <c r="V21" s="6"/>
@@ -53362,7 +53165,7 @@
       <c r="Y21" s="7"/>
       <c r="AA21" t="str">
         <f t="shared" si="0"/>
-        <v>1234567891011121314151617181920</v>
+        <v xml:space="preserve">1234567891011121314151617   </v>
       </c>
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.25">
@@ -53517,12 +53320,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="47" priority="2">
+    <cfRule type="expression" dxfId="118" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="46" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -53535,8 +53338,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AA20" sqref="AA1:AA20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -53564,10 +53367,10 @@
         <v>6</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="H1" s="12" t="s">
         <v>6</v>
@@ -53585,13 +53388,13 @@
         <v>6</v>
       </c>
       <c r="M1" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="N1" s="12" t="s">
         <v>6</v>
       </c>
       <c r="O1" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="P1" s="12" t="s">
         <v>6</v>
@@ -53600,13 +53403,13 @@
         <v>6</v>
       </c>
       <c r="R1" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="S1" s="12" t="s">
         <v>6</v>
       </c>
       <c r="T1" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="U1" s="2"/>
       <c r="V1" s="2"/>
@@ -53619,11 +53422,11 @@
       </c>
       <c r="AA1" t="str">
         <f>CONCATENATE(A1,B1,C1,D1,E1,F1,G1,H1,I1,J1,K1,L1,M1,N1,O1,P1,Q1,R1,S1,T1,U1,V1,W1,X1,Y1)</f>
-        <v>*    *        *    *</v>
+        <v xml:space="preserve">*     *     *    *  </v>
       </c>
       <c r="AB1" t="str">
         <f>"'"&amp;AA1&amp;"',"</f>
-        <v>'*    *        *    *',</v>
+        <v>'*     *     *    *  ',</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
@@ -53646,7 +53449,7 @@
         <v>6</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>6</v>
+        <v>265</v>
       </c>
       <c r="H2" s="12" t="s">
         <v>6</v>
@@ -53698,11 +53501,11 @@
       </c>
       <c r="AA2" t="str">
         <f t="shared" ref="AA2:AA25" si="0">CONCATENATE(A2,B2,C2,D2,E2,F2,G2,H2,I2,J2,K2,L2,M2,N2,O2,P2,Q2,R2,S2,T2,U2,V2,W2,X2,Y2)</f>
-        <v xml:space="preserve">                    </v>
+        <v xml:space="preserve">      i             </v>
       </c>
       <c r="AB2" t="str">
         <f t="shared" ref="AB2:AB20" si="1">"'"&amp;AA2&amp;"',"</f>
-        <v>'                    ',</v>
+        <v>'      i             ',</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
@@ -53725,7 +53528,7 @@
         <v>6</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>6</v>
+        <v>265</v>
       </c>
       <c r="H3" s="12" t="s">
         <v>6</v>
@@ -53777,11 +53580,11 @@
       </c>
       <c r="AA3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">                    </v>
+        <v xml:space="preserve">      i             </v>
       </c>
       <c r="AB3" t="str">
         <f t="shared" si="1"/>
-        <v>'                    ',</v>
+        <v>'      i             ',</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
@@ -53804,7 +53607,7 @@
         <v>6</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>6</v>
+        <v>265</v>
       </c>
       <c r="H4" s="12" t="s">
         <v>6</v>
@@ -53856,11 +53659,11 @@
       </c>
       <c r="AA4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">                    </v>
+        <v xml:space="preserve">      i             </v>
       </c>
       <c r="AB4" t="str">
         <f t="shared" si="1"/>
-        <v>'                    ',</v>
+        <v>'      i             ',</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
@@ -53883,7 +53686,7 @@
         <v>6</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>6</v>
+        <v>265</v>
       </c>
       <c r="H5" s="12" t="s">
         <v>6</v>
@@ -53935,16 +53738,16 @@
       </c>
       <c r="AA5" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">                    </v>
+        <v xml:space="preserve">      i             </v>
       </c>
       <c r="AB5" t="str">
         <f t="shared" si="1"/>
-        <v>'                    ',</v>
+        <v>'      i             ',</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>6</v>
@@ -53959,10 +53762,10 @@
         <v>6</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>6</v>
+        <v>265</v>
       </c>
       <c r="H6" s="12" t="s">
         <v>6</v>
@@ -53986,7 +53789,7 @@
         <v>6</v>
       </c>
       <c r="O6" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="P6" s="12" t="s">
         <v>6</v>
@@ -54001,7 +53804,7 @@
         <v>6</v>
       </c>
       <c r="T6" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="U6" s="6"/>
       <c r="V6" s="6"/>
@@ -54014,34 +53817,34 @@
       </c>
       <c r="AA6" t="str">
         <f t="shared" si="0"/>
-        <v>*    *        *    *</v>
+        <v xml:space="preserve">      i             </v>
       </c>
       <c r="AB6" t="str">
         <f t="shared" si="1"/>
-        <v>'*    *        *    *',</v>
+        <v>'      i             ',</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>6</v>
+        <v>265</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>6</v>
+        <v>265</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>6</v>
+        <v>265</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>6</v>
+        <v>265</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>6</v>
+        <v>265</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="H7" s="12" t="s">
         <v>6</v>
@@ -54059,7 +53862,7 @@
         <v>6</v>
       </c>
       <c r="M7" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="N7" s="12" t="s">
         <v>6</v>
@@ -54074,7 +53877,7 @@
         <v>6</v>
       </c>
       <c r="R7" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="S7" s="12" t="s">
         <v>6</v>
@@ -54093,11 +53896,11 @@
       </c>
       <c r="AA7" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">                    </v>
+        <v xml:space="preserve">*iiiii*     *    *  </v>
       </c>
       <c r="AB7" t="str">
         <f t="shared" si="1"/>
-        <v>'                    ',</v>
+        <v>'*iiiii*     *    *  ',</v>
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
@@ -54418,22 +54221,22 @@
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>6</v>
+        <v>264</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>6</v>
+        <v>264</v>
       </c>
       <c r="G12" s="12" t="s">
         <v>6</v>
@@ -54451,7 +54254,7 @@
         <v>6</v>
       </c>
       <c r="L12" s="12" t="s">
-        <v>6</v>
+        <v>201</v>
       </c>
       <c r="M12" s="12" t="s">
         <v>6</v>
@@ -54466,7 +54269,7 @@
         <v>6</v>
       </c>
       <c r="Q12" s="12" t="s">
-        <v>6</v>
+        <v>201</v>
       </c>
       <c r="R12" s="12" t="s">
         <v>6</v>
@@ -54488,31 +54291,31 @@
       </c>
       <c r="AA12" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">                    </v>
+        <v xml:space="preserve">H****H     p    p   </v>
       </c>
       <c r="AB12" t="str">
         <f t="shared" si="1"/>
-        <v>'                    ',</v>
+        <v>'H****H     p    p   ',</v>
       </c>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="G13" s="12" t="s">
         <v>6</v>
@@ -54567,31 +54370,31 @@
       </c>
       <c r="AA13" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">                    </v>
+        <v xml:space="preserve">******              </v>
       </c>
       <c r="AB13" t="str">
         <f t="shared" si="1"/>
-        <v>'                    ',</v>
+        <v>'******              ',</v>
       </c>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="G14" s="12" t="s">
         <v>6</v>
@@ -54646,11 +54449,11 @@
       </c>
       <c r="AA14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">                    </v>
+        <v xml:space="preserve">******              </v>
       </c>
       <c r="AB14" t="str">
         <f t="shared" si="1"/>
-        <v>'                    ',</v>
+        <v>'******              ',</v>
       </c>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.25">
@@ -54697,13 +54500,13 @@
         <v>6</v>
       </c>
       <c r="O15" s="12" t="s">
-        <v>201</v>
+        <v>6</v>
       </c>
       <c r="P15" s="12" t="s">
         <v>6</v>
       </c>
       <c r="Q15" s="12" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="R15" s="12" t="s">
         <v>6</v>
@@ -54712,7 +54515,7 @@
         <v>6</v>
       </c>
       <c r="T15" s="12" t="s">
-        <v>201</v>
+        <v>6</v>
       </c>
       <c r="U15" s="6"/>
       <c r="V15" s="6"/>
@@ -54725,11 +54528,11 @@
       </c>
       <c r="AA15" t="str">
         <f t="shared" si="0"/>
-        <v>******        p    p</v>
+        <v xml:space="preserve">******          T   </v>
       </c>
       <c r="AB15" t="str">
         <f t="shared" si="1"/>
-        <v>'******        p    p',</v>
+        <v>'******          T   ',</v>
       </c>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.25">
@@ -54813,7 +54616,7 @@
     </row>
     <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>61</v>
+        <v>264</v>
       </c>
       <c r="B17" s="12" t="s">
         <v>61</v>
@@ -54828,7 +54631,7 @@
         <v>61</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>61</v>
+        <v>264</v>
       </c>
       <c r="G17" s="12" t="s">
         <v>6</v>
@@ -54846,7 +54649,7 @@
         <v>6</v>
       </c>
       <c r="L17" s="12" t="s">
-        <v>6</v>
+        <v>201</v>
       </c>
       <c r="M17" s="12" t="s">
         <v>6</v>
@@ -54861,7 +54664,7 @@
         <v>6</v>
       </c>
       <c r="Q17" s="12" t="s">
-        <v>6</v>
+        <v>201</v>
       </c>
       <c r="R17" s="12" t="s">
         <v>6</v>
@@ -54883,31 +54686,31 @@
       </c>
       <c r="AA17" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">******              </v>
+        <v xml:space="preserve">H****H     p    p   </v>
       </c>
       <c r="AB17" t="str">
         <f t="shared" si="1"/>
-        <v>'******              ',</v>
+        <v>'H****H     p    p   ',</v>
       </c>
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="G18" s="12" t="s">
         <v>6</v>
@@ -54949,7 +54752,7 @@
         <v>6</v>
       </c>
       <c r="T18" s="12" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="U18" s="6"/>
       <c r="V18" s="6"/>
@@ -54962,31 +54765,31 @@
       </c>
       <c r="AA18" t="str">
         <f t="shared" si="0"/>
-        <v>******             T</v>
+        <v xml:space="preserve">                    </v>
       </c>
       <c r="AB18" t="str">
         <f t="shared" si="1"/>
-        <v>'******             T',</v>
+        <v>'                    ',</v>
       </c>
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="G19" s="12" t="s">
         <v>6</v>
@@ -55041,31 +54844,31 @@
       </c>
       <c r="AA19" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">******              </v>
+        <v xml:space="preserve">                    </v>
       </c>
       <c r="AB19" t="str">
         <f t="shared" si="1"/>
-        <v>'******              ',</v>
+        <v>'                    ',</v>
       </c>
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="G20" s="12" t="s">
         <v>6</v>
@@ -55092,7 +54895,7 @@
         <v>6</v>
       </c>
       <c r="O20" s="12" t="s">
-        <v>201</v>
+        <v>6</v>
       </c>
       <c r="P20" s="12" t="s">
         <v>6</v>
@@ -55107,7 +54910,7 @@
         <v>6</v>
       </c>
       <c r="T20" s="12" t="s">
-        <v>201</v>
+        <v>6</v>
       </c>
       <c r="U20" s="6"/>
       <c r="V20" s="6"/>
@@ -55120,11 +54923,11 @@
       </c>
       <c r="AA20" t="str">
         <f t="shared" si="0"/>
-        <v>******        p    p</v>
+        <v xml:space="preserve">                    </v>
       </c>
       <c r="AB20" t="str">
         <f t="shared" si="1"/>
-        <v>'******        p    p',</v>
+        <v>'                    ',</v>
       </c>
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.25">
@@ -55369,43 +55172,43 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A7:Y14 A21:Y25 G15:Y20 G1:N6 U1:Y6">
-    <cfRule type="expression" dxfId="79" priority="8">
+  <conditionalFormatting sqref="A7:Y14 A21:Y25 G1:N6 G6:G7 S1:Y6 M5:N7 L12:Q17 G15:Y20 A18:F20">
+    <cfRule type="expression" dxfId="116" priority="8">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A7:Z14 A21:Z25 G15:Z20 G1:N6 U1:Z6">
-    <cfRule type="cellIs" dxfId="78" priority="7" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="A7:Z14 A21:Z25 G1:N6 G6:G7 S1:Z6 M5:N7 L12:Q17 G15:Z20 A18:F20">
+    <cfRule type="cellIs" dxfId="115" priority="7" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A15:F20">
-    <cfRule type="expression" dxfId="67" priority="6">
+  <conditionalFormatting sqref="A12:F17">
+    <cfRule type="expression" dxfId="114" priority="6">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A15:F20">
-    <cfRule type="cellIs" dxfId="66" priority="5" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="A12:F17">
+    <cfRule type="cellIs" dxfId="113" priority="5" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O1:T6">
-    <cfRule type="expression" dxfId="45" priority="4">
+  <conditionalFormatting sqref="M1:R7">
+    <cfRule type="expression" dxfId="112" priority="4">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O1:T6">
-    <cfRule type="cellIs" dxfId="43" priority="3" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="M1:R7">
+    <cfRule type="cellIs" dxfId="111" priority="3" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:F6">
-    <cfRule type="expression" dxfId="41" priority="2">
+  <conditionalFormatting sqref="A1:G7">
+    <cfRule type="expression" dxfId="110" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:F6">
-    <cfRule type="cellIs" dxfId="39" priority="1" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="A1:G7">
+    <cfRule type="cellIs" dxfId="109" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -55419,7 +55222,7 @@
   <dimension ref="A1:AB30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AA20" sqref="AA1:AA20"/>
+      <selection activeCell="B39" sqref="B39:C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -55447,10 +55250,10 @@
         <v>6</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="H1" s="12" t="s">
         <v>6</v>
@@ -55468,13 +55271,13 @@
         <v>6</v>
       </c>
       <c r="M1" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="N1" s="12" t="s">
         <v>6</v>
       </c>
       <c r="O1" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="P1" s="12" t="s">
         <v>6</v>
@@ -55483,13 +55286,13 @@
         <v>6</v>
       </c>
       <c r="R1" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="S1" s="12" t="s">
         <v>6</v>
       </c>
       <c r="T1" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="U1" s="2"/>
       <c r="V1" s="2"/>
@@ -55500,12 +55303,13 @@
         <f>ROW()</f>
         <v>1</v>
       </c>
-      <c r="AA1" t="s">
-        <v>287</v>
+      <c r="AA1" t="str">
+        <f>CONCATENATE(A1,B1,C1,D1,E1,F1,G1,H1,I1,J1,K1,L1,M1,N1,O1,P1,Q1,R1,S1,T1,U1,V1,W1,X1,Y1)</f>
+        <v xml:space="preserve">*     *     *    *  </v>
       </c>
       <c r="AB1" t="str">
         <f>"'"&amp;AA1&amp;"',"</f>
-        <v>'*    *        *    *',</v>
+        <v>'*     *     *    *  ',</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
@@ -55528,7 +55332,7 @@
         <v>6</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>6</v>
+        <v>265</v>
       </c>
       <c r="H2" s="12" t="s">
         <v>6</v>
@@ -55578,12 +55382,13 @@
         <f>ROW()</f>
         <v>2</v>
       </c>
-      <c r="AA2" t="s">
-        <v>288</v>
+      <c r="AA2" t="str">
+        <f t="shared" ref="AA2:AA20" si="0">CONCATENATE(A2,B2,C2,D2,E2,F2,G2,H2,I2,J2,K2,L2,M2,N2,O2,P2,Q2,R2,S2,T2,U2,V2,W2,X2,Y2)</f>
+        <v xml:space="preserve">      i             </v>
       </c>
       <c r="AB2" t="str">
-        <f t="shared" ref="AB2:AB20" si="0">"'"&amp;AA2&amp;"',"</f>
-        <v>'                    ',</v>
+        <f t="shared" ref="AB2:AB20" si="1">"'"&amp;AA2&amp;"',"</f>
+        <v>'      i             ',</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
@@ -55606,7 +55411,7 @@
         <v>6</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>6</v>
+        <v>265</v>
       </c>
       <c r="H3" s="12" t="s">
         <v>6</v>
@@ -55656,12 +55461,13 @@
         <f>ROW()</f>
         <v>3</v>
       </c>
-      <c r="AA3" t="s">
-        <v>288</v>
+      <c r="AA3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">      i             </v>
       </c>
       <c r="AB3" t="str">
-        <f t="shared" si="0"/>
-        <v>'                    ',</v>
+        <f t="shared" si="1"/>
+        <v>'      i             ',</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
@@ -55684,7 +55490,7 @@
         <v>6</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>6</v>
+        <v>265</v>
       </c>
       <c r="H4" s="12" t="s">
         <v>6</v>
@@ -55734,12 +55540,13 @@
         <f>ROW()</f>
         <v>4</v>
       </c>
-      <c r="AA4" t="s">
-        <v>288</v>
+      <c r="AA4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">      i             </v>
       </c>
       <c r="AB4" t="str">
-        <f t="shared" si="0"/>
-        <v>'                    ',</v>
+        <f t="shared" si="1"/>
+        <v>'      i             ',</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
@@ -55762,7 +55569,7 @@
         <v>6</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>6</v>
+        <v>265</v>
       </c>
       <c r="H5" s="12" t="s">
         <v>6</v>
@@ -55812,17 +55619,18 @@
         <f>ROW()</f>
         <v>5</v>
       </c>
-      <c r="AA5" t="s">
-        <v>288</v>
+      <c r="AA5" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">      i             </v>
       </c>
       <c r="AB5" t="str">
-        <f t="shared" si="0"/>
-        <v>'                    ',</v>
+        <f t="shared" si="1"/>
+        <v>'      i             ',</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>6</v>
@@ -55837,10 +55645,10 @@
         <v>6</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>6</v>
+        <v>265</v>
       </c>
       <c r="H6" s="12" t="s">
         <v>6</v>
@@ -55864,7 +55672,7 @@
         <v>6</v>
       </c>
       <c r="O6" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="P6" s="12" t="s">
         <v>6</v>
@@ -55879,7 +55687,7 @@
         <v>6</v>
       </c>
       <c r="T6" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="U6" s="6"/>
       <c r="V6" s="6"/>
@@ -55890,35 +55698,36 @@
         <f>ROW()</f>
         <v>6</v>
       </c>
-      <c r="AA6" t="s">
-        <v>287</v>
+      <c r="AA6" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">      i             </v>
       </c>
       <c r="AB6" t="str">
-        <f t="shared" si="0"/>
-        <v>'*    *        *    *',</v>
+        <f t="shared" si="1"/>
+        <v>'      i             ',</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>6</v>
+        <v>265</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>6</v>
+        <v>265</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>6</v>
+        <v>265</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>6</v>
+        <v>265</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>6</v>
+        <v>265</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="H7" s="12" t="s">
         <v>6</v>
@@ -55936,7 +55745,7 @@
         <v>6</v>
       </c>
       <c r="M7" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="N7" s="12" t="s">
         <v>6</v>
@@ -55951,7 +55760,7 @@
         <v>6</v>
       </c>
       <c r="R7" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="S7" s="12" t="s">
         <v>6</v>
@@ -55968,12 +55777,13 @@
         <f>ROW()</f>
         <v>7</v>
       </c>
-      <c r="AA7" t="s">
-        <v>288</v>
+      <c r="AA7" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">*iiiii*     *    *  </v>
       </c>
       <c r="AB7" t="str">
-        <f t="shared" si="0"/>
-        <v>'                    ',</v>
+        <f t="shared" si="1"/>
+        <v>'*iiiii*     *    *  ',</v>
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
@@ -56046,11 +55856,12 @@
         <f>ROW()</f>
         <v>8</v>
       </c>
-      <c r="AA8" t="s">
-        <v>288</v>
+      <c r="AA8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">                    </v>
       </c>
       <c r="AB8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>'                    ',</v>
       </c>
     </row>
@@ -56124,11 +55935,12 @@
         <f>ROW()</f>
         <v>9</v>
       </c>
-      <c r="AA9" t="s">
-        <v>288</v>
+      <c r="AA9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">                    </v>
       </c>
       <c r="AB9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>'                    ',</v>
       </c>
     </row>
@@ -56202,11 +56014,12 @@
         <f>ROW()</f>
         <v>10</v>
       </c>
-      <c r="AA10" t="s">
-        <v>288</v>
+      <c r="AA10" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">                    </v>
       </c>
       <c r="AB10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>'                    ',</v>
       </c>
     </row>
@@ -56280,20 +56093,21 @@
         <f>ROW()</f>
         <v>11</v>
       </c>
-      <c r="AA11" t="s">
-        <v>288</v>
+      <c r="AA11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">                    </v>
       </c>
       <c r="AB11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>'                    ',</v>
       </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>6</v>
+        <v>201</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C12" s="12" t="s">
         <v>6</v>
@@ -56305,7 +56119,7 @@
         <v>6</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>6</v>
+        <v>201</v>
       </c>
       <c r="G12" s="12" t="s">
         <v>6</v>
@@ -56358,12 +56172,13 @@
         <f>ROW()</f>
         <v>12</v>
       </c>
-      <c r="AA12" t="s">
-        <v>288</v>
+      <c r="AA12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">pT   p              </v>
       </c>
       <c r="AB12" t="str">
-        <f t="shared" si="0"/>
-        <v>'                    ',</v>
+        <f t="shared" si="1"/>
+        <v>'pT   p              ',</v>
       </c>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.25">
@@ -56436,11 +56251,12 @@
         <f>ROW()</f>
         <v>13</v>
       </c>
-      <c r="AA13" t="s">
-        <v>288</v>
+      <c r="AA13" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">                    </v>
       </c>
       <c r="AB13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>'                    ',</v>
       </c>
     </row>
@@ -56514,20 +56330,21 @@
         <f>ROW()</f>
         <v>14</v>
       </c>
-      <c r="AA14" t="s">
-        <v>288</v>
+      <c r="AA14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">                    </v>
       </c>
       <c r="AB14" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>'                    ',</v>
       </c>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>201</v>
+        <v>6</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>6</v>
@@ -56539,7 +56356,7 @@
         <v>6</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>201</v>
+        <v>6</v>
       </c>
       <c r="G15" s="12" t="s">
         <v>6</v>
@@ -56592,12 +56409,13 @@
         <f>ROW()</f>
         <v>15</v>
       </c>
-      <c r="AA15" t="s">
-        <v>289</v>
+      <c r="AA15" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">                    </v>
       </c>
       <c r="AB15" t="str">
-        <f t="shared" si="0"/>
-        <v>'pT   p              ',</v>
+        <f t="shared" si="1"/>
+        <v>'                    ',</v>
       </c>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.25">
@@ -56670,17 +56488,18 @@
         <f>ROW()</f>
         <v>16</v>
       </c>
-      <c r="AA16" t="s">
-        <v>288</v>
+      <c r="AA16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">                    </v>
       </c>
       <c r="AB16" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>'                    ',</v>
       </c>
     </row>
     <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>6</v>
+        <v>201</v>
       </c>
       <c r="B17" s="12" t="s">
         <v>6</v>
@@ -56695,7 +56514,7 @@
         <v>6</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>6</v>
+        <v>201</v>
       </c>
       <c r="G17" s="12" t="s">
         <v>6</v>
@@ -56748,12 +56567,13 @@
         <f>ROW()</f>
         <v>17</v>
       </c>
-      <c r="AA17" t="s">
-        <v>288</v>
+      <c r="AA17" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">p    p              </v>
       </c>
       <c r="AB17" t="str">
-        <f t="shared" si="0"/>
-        <v>'                    ',</v>
+        <f t="shared" si="1"/>
+        <v>'p    p              ',</v>
       </c>
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.25">
@@ -56826,11 +56646,12 @@
         <f>ROW()</f>
         <v>18</v>
       </c>
-      <c r="AA18" t="s">
-        <v>288</v>
+      <c r="AA18" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">                    </v>
       </c>
       <c r="AB18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>'                    ',</v>
       </c>
     </row>
@@ -56904,17 +56725,18 @@
         <f>ROW()</f>
         <v>19</v>
       </c>
-      <c r="AA19" t="s">
-        <v>288</v>
+      <c r="AA19" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">                    </v>
       </c>
       <c r="AB19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>'                    ',</v>
       </c>
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
-        <v>201</v>
+        <v>6</v>
       </c>
       <c r="B20" s="12" t="s">
         <v>6</v>
@@ -56929,7 +56751,7 @@
         <v>6</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>201</v>
+        <v>6</v>
       </c>
       <c r="G20" s="12" t="s">
         <v>6</v>
@@ -56982,12 +56804,13 @@
         <f>ROW()</f>
         <v>20</v>
       </c>
-      <c r="AA20" t="s">
-        <v>290</v>
+      <c r="AA20" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">                    </v>
       </c>
       <c r="AB20" t="str">
-        <f t="shared" si="0"/>
-        <v>'p    p              ',</v>
+        <f t="shared" si="1"/>
+        <v>'                    ',</v>
       </c>
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.25">
@@ -57077,7 +56900,7 @@
       <c r="X21" s="6"/>
       <c r="Y21" s="7"/>
       <c r="AA21" t="str">
-        <f t="shared" ref="AA2:AA25" si="1">CONCATENATE(A21,B21,C21,D21,E21,F21,G21,H21,I21,J21,K21,L21,M21,N21,O21,P21,Q21,R21,S21,T21,U21,V21,W21,X21,Y21)</f>
+        <f t="shared" ref="AA21:AA25" si="2">CONCATENATE(A21,B21,C21,D21,E21,F21,G21,H21,I21,J21,K21,L21,M21,N21,O21,P21,Q21,R21,S21,T21,U21,V21,W21,X21,Y21)</f>
         <v>1234567891011121314151617181920</v>
       </c>
     </row>
@@ -57108,7 +56931,7 @@
       <c r="X22" s="6"/>
       <c r="Y22" s="7"/>
       <c r="AA22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -57139,7 +56962,7 @@
       <c r="X23" s="6"/>
       <c r="Y23" s="7"/>
       <c r="AA23" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -57170,7 +56993,7 @@
       <c r="X24" s="6"/>
       <c r="Y24" s="7"/>
       <c r="AA24" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -57201,7 +57024,7 @@
       <c r="X25" s="10"/>
       <c r="Y25" s="11"/>
       <c r="AA25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -57232,33 +57055,63 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F1:N5 A6:N6 U1:Y6 A7:Y25">
-    <cfRule type="expression" dxfId="73" priority="8">
+  <conditionalFormatting sqref="U1:Y6 F1:N5 A6:N6 A7:Y25 M1:O7">
+    <cfRule type="expression" dxfId="108" priority="14">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:N5 A6:N6 U1:Z6 A7:Z25">
-    <cfRule type="cellIs" dxfId="72" priority="7" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="U1:Z6 F1:N5 A6:N6 A7:Z25 M1:O7">
+    <cfRule type="cellIs" dxfId="107" priority="13" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:E5">
-    <cfRule type="expression" dxfId="63" priority="4">
+    <cfRule type="expression" dxfId="106" priority="10">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:E5">
-    <cfRule type="cellIs" dxfId="62" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="9" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O1:T6">
-    <cfRule type="expression" dxfId="31" priority="2">
+  <conditionalFormatting sqref="L1:T6 M6:R7">
+    <cfRule type="expression" dxfId="104" priority="8">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O1:T6">
-    <cfRule type="cellIs" dxfId="29" priority="1" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="L1:T6 M6:R7">
+    <cfRule type="cellIs" dxfId="103" priority="7" stopIfTrue="1" operator="equal">
+      <formula>":"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:F5">
+    <cfRule type="expression" dxfId="23" priority="6">
+      <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:F5">
+    <cfRule type="cellIs" dxfId="22" priority="5" stopIfTrue="1" operator="equal">
+      <formula>":"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A6:E6">
+    <cfRule type="expression" dxfId="21" priority="4">
+      <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A6:E6">
+    <cfRule type="cellIs" dxfId="20" priority="3" stopIfTrue="1" operator="equal">
+      <formula>":"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F6">
+    <cfRule type="expression" dxfId="19" priority="2">
+      <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F6">
+    <cfRule type="cellIs" dxfId="18" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -57300,10 +57153,10 @@
         <v>6</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="H1" s="12" t="s">
         <v>6</v>
@@ -57321,10 +57174,10 @@
         <v>6</v>
       </c>
       <c r="M1" s="12" t="s">
-        <v>6</v>
+        <v>264</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="O1" s="12" t="s">
         <v>61</v>
@@ -57336,13 +57189,13 @@
         <v>61</v>
       </c>
       <c r="R1" s="12" t="s">
-        <v>61</v>
+        <v>264</v>
       </c>
       <c r="S1" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="T1" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="U1" s="2"/>
       <c r="V1" s="2"/>
@@ -57355,11 +57208,11 @@
       </c>
       <c r="AA1" t="str">
         <f>CONCATENATE(A1,B1,C1,D1,E1,F1,G1,H1,I1,J1,K1,L1,M1,N1,O1,P1,Q1,R1,S1,T1,U1,V1,W1,X1,Y1)</f>
-        <v>*    *        ******</v>
+        <v xml:space="preserve">*     *     H****H  </v>
       </c>
       <c r="AB1" t="str">
         <f>"'"&amp;AA1&amp;"',"</f>
-        <v>'*    *        ******',</v>
+        <v>'*     *     H****H  ',</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
@@ -57382,7 +57235,7 @@
         <v>6</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>6</v>
+        <v>265</v>
       </c>
       <c r="H2" s="12" t="s">
         <v>6</v>
@@ -57400,10 +57253,10 @@
         <v>6</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="N2" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="O2" s="12" t="s">
         <v>61</v>
@@ -57418,10 +57271,10 @@
         <v>61</v>
       </c>
       <c r="S2" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="T2" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="U2" s="6"/>
       <c r="V2" s="6"/>
@@ -57434,11 +57287,11 @@
       </c>
       <c r="AA2" t="str">
         <f t="shared" ref="AA2:AA25" si="0">CONCATENATE(A2,B2,C2,D2,E2,F2,G2,H2,I2,J2,K2,L2,M2,N2,O2,P2,Q2,R2,S2,T2,U2,V2,W2,X2,Y2)</f>
-        <v xml:space="preserve">              ******</v>
+        <v xml:space="preserve">      i     ******  </v>
       </c>
       <c r="AB2" t="str">
         <f t="shared" ref="AB2:AB20" si="1">"'"&amp;AA2&amp;"',"</f>
-        <v>'              ******',</v>
+        <v>'      i     ******  ',</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
@@ -57461,7 +57314,7 @@
         <v>6</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>6</v>
+        <v>265</v>
       </c>
       <c r="H3" s="12" t="s">
         <v>6</v>
@@ -57479,10 +57332,10 @@
         <v>6</v>
       </c>
       <c r="M3" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="N3" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="O3" s="12" t="s">
         <v>61</v>
@@ -57497,10 +57350,10 @@
         <v>61</v>
       </c>
       <c r="S3" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="T3" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="U3" s="6"/>
       <c r="V3" s="6"/>
@@ -57513,11 +57366,11 @@
       </c>
       <c r="AA3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">              ******</v>
+        <v xml:space="preserve">      i     ******  </v>
       </c>
       <c r="AB3" t="str">
         <f t="shared" si="1"/>
-        <v>'              ******',</v>
+        <v>'      i     ******  ',</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
@@ -57540,7 +57393,7 @@
         <v>6</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>6</v>
+        <v>265</v>
       </c>
       <c r="H4" s="12" t="s">
         <v>6</v>
@@ -57558,10 +57411,10 @@
         <v>6</v>
       </c>
       <c r="M4" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="N4" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="O4" s="12" t="s">
         <v>61</v>
@@ -57576,10 +57429,10 @@
         <v>61</v>
       </c>
       <c r="S4" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="T4" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="U4" s="6"/>
       <c r="V4" s="6"/>
@@ -57592,11 +57445,11 @@
       </c>
       <c r="AA4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">              ******</v>
+        <v xml:space="preserve">      i     ******  </v>
       </c>
       <c r="AB4" t="str">
         <f t="shared" si="1"/>
-        <v>'              ******',</v>
+        <v>'      i     ******  ',</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
@@ -57619,7 +57472,7 @@
         <v>6</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>6</v>
+        <v>265</v>
       </c>
       <c r="H5" s="12" t="s">
         <v>6</v>
@@ -57637,10 +57490,10 @@
         <v>6</v>
       </c>
       <c r="M5" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="N5" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="O5" s="12" t="s">
         <v>61</v>
@@ -57655,10 +57508,10 @@
         <v>61</v>
       </c>
       <c r="S5" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="T5" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="U5" s="6"/>
       <c r="V5" s="6"/>
@@ -57671,16 +57524,16 @@
       </c>
       <c r="AA5" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">              ******</v>
+        <v xml:space="preserve">      i     ******  </v>
       </c>
       <c r="AB5" t="str">
         <f t="shared" si="1"/>
-        <v>'              ******',</v>
+        <v>'      i     ******  ',</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>6</v>
@@ -57695,10 +57548,10 @@
         <v>6</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>6</v>
+        <v>265</v>
       </c>
       <c r="H6" s="12" t="s">
         <v>6</v>
@@ -57716,10 +57569,10 @@
         <v>6</v>
       </c>
       <c r="M6" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="N6" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="O6" s="12" t="s">
         <v>61</v>
@@ -57734,10 +57587,10 @@
         <v>61</v>
       </c>
       <c r="S6" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="T6" s="12" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="U6" s="6"/>
       <c r="V6" s="6"/>
@@ -57750,34 +57603,34 @@
       </c>
       <c r="AA6" t="str">
         <f t="shared" si="0"/>
-        <v>*    *        ******</v>
+        <v xml:space="preserve">      i     ******  </v>
       </c>
       <c r="AB6" t="str">
         <f t="shared" si="1"/>
-        <v>'*    *        ******',</v>
+        <v>'      i     ******  ',</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>6</v>
+        <v>265</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>6</v>
+        <v>265</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>6</v>
+        <v>265</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>6</v>
+        <v>265</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>6</v>
+        <v>265</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="H7" s="12" t="s">
         <v>6</v>
@@ -57795,22 +57648,22 @@
         <v>6</v>
       </c>
       <c r="M7" s="12" t="s">
-        <v>6</v>
+        <v>264</v>
       </c>
       <c r="N7" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="O7" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="P7" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="Q7" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="R7" s="12" t="s">
-        <v>6</v>
+        <v>264</v>
       </c>
       <c r="S7" s="12" t="s">
         <v>6</v>
@@ -57829,11 +57682,11 @@
       </c>
       <c r="AA7" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">                    </v>
+        <v xml:space="preserve">*iiiii*     H****H  </v>
       </c>
       <c r="AB7" t="str">
         <f t="shared" si="1"/>
-        <v>'                    ',</v>
+        <v>'*iiiii*     H****H  ',</v>
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
@@ -59105,63 +58958,143 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A7:Y25 F2:N5 B6:E6 U1:Y6 G1:N1 G6:N6">
-    <cfRule type="expression" dxfId="81" priority="12">
+  <conditionalFormatting sqref="A8:Y25 G1:N1 S1:Y7 F2:N5 B6:N6 A7:N7">
+    <cfRule type="expression" dxfId="102" priority="28">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A7:Z25 F2:N5 B6:E6 U1:Z6 G1:N1 G6:N6">
-    <cfRule type="cellIs" dxfId="80" priority="11" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="A8:Z25 G1:N1 S1:Z7 F2:N5 B6:N6 A7:N7">
+    <cfRule type="cellIs" dxfId="101" priority="27" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:E5">
-    <cfRule type="expression" dxfId="69" priority="10">
+    <cfRule type="expression" dxfId="100" priority="26">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:E5">
-    <cfRule type="cellIs" dxfId="68" priority="9" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="25" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O1:T6">
-    <cfRule type="expression" dxfId="65" priority="8">
+  <conditionalFormatting sqref="M1:R7">
+    <cfRule type="expression" dxfId="98" priority="24">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O1:T6">
-    <cfRule type="cellIs" dxfId="64" priority="7" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="M1:R7">
+    <cfRule type="cellIs" dxfId="97" priority="23" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6">
-    <cfRule type="expression" dxfId="21" priority="6">
+    <cfRule type="expression" dxfId="96" priority="22">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6">
-    <cfRule type="cellIs" dxfId="19" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="21" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1">
-    <cfRule type="expression" dxfId="17" priority="4">
+    <cfRule type="expression" dxfId="94" priority="20">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1">
-    <cfRule type="cellIs" dxfId="15" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="19" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6">
-    <cfRule type="expression" dxfId="13" priority="2">
+    <cfRule type="expression" dxfId="92" priority="18">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6">
-    <cfRule type="cellIs" dxfId="11" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="17" stopIfTrue="1" operator="equal">
+      <formula>":"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:F5">
+    <cfRule type="expression" dxfId="17" priority="16">
+      <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:F5">
+    <cfRule type="cellIs" dxfId="16" priority="15" stopIfTrue="1" operator="equal">
+      <formula>":"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G1">
+    <cfRule type="expression" dxfId="15" priority="14">
+      <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G1">
+    <cfRule type="cellIs" dxfId="14" priority="13" stopIfTrue="1" operator="equal">
+      <formula>":"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G6">
+    <cfRule type="expression" dxfId="13" priority="12">
+      <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G6">
+    <cfRule type="cellIs" dxfId="12" priority="11" stopIfTrue="1" operator="equal">
+      <formula>":"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A6:E6">
+    <cfRule type="expression" dxfId="11" priority="10">
+      <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A6:E6">
+    <cfRule type="cellIs" dxfId="10" priority="9" stopIfTrue="1" operator="equal">
+      <formula>":"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A7">
+    <cfRule type="expression" dxfId="9" priority="8">
+      <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A7">
+    <cfRule type="cellIs" dxfId="8" priority="7" stopIfTrue="1" operator="equal">
+      <formula>":"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F7">
+    <cfRule type="expression" dxfId="7" priority="6">
+      <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F7">
+    <cfRule type="cellIs" dxfId="6" priority="5" stopIfTrue="1" operator="equal">
+      <formula>":"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F6">
+    <cfRule type="expression" dxfId="5" priority="4">
+      <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F6">
+    <cfRule type="cellIs" dxfId="4" priority="3" stopIfTrue="1" operator="equal">
+      <formula>":"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G7">
+    <cfRule type="expression" dxfId="3" priority="2">
+      <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G7">
+    <cfRule type="cellIs" dxfId="2" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -59188,7 +59121,7 @@
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>61</v>
+        <v>264</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>61</v>
@@ -59206,7 +59139,7 @@
         <v>61</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>6</v>
+        <v>264</v>
       </c>
       <c r="H1" s="12" t="s">
         <v>6</v>
@@ -59224,28 +59157,28 @@
         <v>6</v>
       </c>
       <c r="M1" s="12" t="s">
-        <v>6</v>
+        <v>201</v>
       </c>
       <c r="N1" s="12" t="s">
         <v>6</v>
       </c>
       <c r="O1" s="12" t="s">
+        <v>286</v>
+      </c>
+      <c r="P1" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q1" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="R1" s="12" t="s">
         <v>201</v>
       </c>
-      <c r="P1" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q1" s="12" t="s">
-        <v>286</v>
-      </c>
-      <c r="R1" s="12" t="s">
-        <v>6</v>
-      </c>
       <c r="S1" s="12" t="s">
         <v>6</v>
       </c>
       <c r="T1" s="12" t="s">
-        <v>201</v>
+        <v>6</v>
       </c>
       <c r="U1" s="2"/>
       <c r="V1" s="2"/>
@@ -59258,11 +59191,11 @@
       </c>
       <c r="AA1" t="str">
         <f>CONCATENATE(A1,B1,C1,D1,E1,F1,G1,H1,I1,J1,K1,L1,M1,N1,O1,P1,Q1,R1,S1,T1,U1,V1,W1,X1,Y1)</f>
-        <v>******        p t  p</v>
+        <v xml:space="preserve">H*****H     p t  p  </v>
       </c>
       <c r="AB1" t="str">
         <f>"'"&amp;AA1&amp;"',"</f>
-        <v>'******        p t  p',</v>
+        <v>'H*****H     p t  p  ',</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
@@ -59285,7 +59218,7 @@
         <v>61</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="H2" s="12" t="s">
         <v>6</v>
@@ -59337,11 +59270,11 @@
       </c>
       <c r="AA2" t="str">
         <f t="shared" ref="AA2:AA25" si="0">CONCATENATE(A2,B2,C2,D2,E2,F2,G2,H2,I2,J2,K2,L2,M2,N2,O2,P2,Q2,R2,S2,T2,U2,V2,W2,X2,Y2)</f>
-        <v xml:space="preserve">******              </v>
+        <v xml:space="preserve">*******             </v>
       </c>
       <c r="AB2" t="str">
         <f t="shared" ref="AB2:AB20" si="1">"'"&amp;AA2&amp;"',"</f>
-        <v>'******              ',</v>
+        <v>'*******             ',</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
@@ -59364,7 +59297,7 @@
         <v>61</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="H3" s="12" t="s">
         <v>6</v>
@@ -59416,11 +59349,11 @@
       </c>
       <c r="AA3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">******              </v>
+        <v xml:space="preserve">*******             </v>
       </c>
       <c r="AB3" t="str">
         <f t="shared" si="1"/>
-        <v>'******              ',</v>
+        <v>'*******             ',</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
@@ -59443,7 +59376,7 @@
         <v>61</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="H4" s="12" t="s">
         <v>6</v>
@@ -59495,11 +59428,11 @@
       </c>
       <c r="AA4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">******              </v>
+        <v xml:space="preserve">*******             </v>
       </c>
       <c r="AB4" t="str">
         <f t="shared" si="1"/>
-        <v>'******              ',</v>
+        <v>'*******             ',</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
@@ -59522,7 +59455,7 @@
         <v>61</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="H5" s="12" t="s">
         <v>6</v>
@@ -59574,11 +59507,11 @@
       </c>
       <c r="AA5" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">******              </v>
+        <v xml:space="preserve">*******             </v>
       </c>
       <c r="AB5" t="str">
         <f t="shared" si="1"/>
-        <v>'******              ',</v>
+        <v>'*******             ',</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
@@ -59601,7 +59534,7 @@
         <v>61</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="H6" s="12" t="s">
         <v>6</v>
@@ -59625,7 +59558,7 @@
         <v>6</v>
       </c>
       <c r="O6" s="12" t="s">
-        <v>201</v>
+        <v>6</v>
       </c>
       <c r="P6" s="12" t="s">
         <v>6</v>
@@ -59640,7 +59573,7 @@
         <v>6</v>
       </c>
       <c r="T6" s="12" t="s">
-        <v>201</v>
+        <v>6</v>
       </c>
       <c r="U6" s="6"/>
       <c r="V6" s="6"/>
@@ -59653,34 +59586,34 @@
       </c>
       <c r="AA6" t="str">
         <f t="shared" si="0"/>
-        <v>******        p    p</v>
+        <v xml:space="preserve">*******             </v>
       </c>
       <c r="AB6" t="str">
         <f t="shared" si="1"/>
-        <v>'******        p    p',</v>
+        <v>'*******             ',</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>6</v>
+        <v>264</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>6</v>
+        <v>264</v>
       </c>
       <c r="H7" s="12" t="s">
         <v>6</v>
@@ -59698,7 +59631,7 @@
         <v>6</v>
       </c>
       <c r="M7" s="12" t="s">
-        <v>6</v>
+        <v>201</v>
       </c>
       <c r="N7" s="12" t="s">
         <v>6</v>
@@ -59713,7 +59646,7 @@
         <v>6</v>
       </c>
       <c r="R7" s="12" t="s">
-        <v>6</v>
+        <v>201</v>
       </c>
       <c r="S7" s="12" t="s">
         <v>6</v>
@@ -59732,11 +59665,11 @@
       </c>
       <c r="AA7" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">                    </v>
+        <v xml:space="preserve">H*****H     p    p  </v>
       </c>
       <c r="AB7" t="str">
         <f t="shared" si="1"/>
-        <v>'                    ',</v>
+        <v>'H*****H     p    p  ',</v>
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
@@ -61009,12 +60942,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="83" priority="2">
+    <cfRule type="expression" dxfId="90" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="82" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -61028,7 +60961,7 @@
   <dimension ref="A1:AB30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AA20" sqref="AA1:AA20"/>
+      <selection activeCell="V33" sqref="V33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -61056,10 +60989,10 @@
         <v>6</v>
       </c>
       <c r="F1" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="12" t="s">
         <v>201</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>6</v>
       </c>
       <c r="H1" s="12" t="s">
         <v>6</v>
@@ -61111,11 +61044,11 @@
       </c>
       <c r="AA1" t="str">
         <f>CONCATENATE(A1,B1,C1,D1,E1,F1,G1,H1,I1,J1,K1,L1,M1,N1,O1,P1,Q1,R1,S1,T1,U1,V1,W1,X1,Y1)</f>
-        <v xml:space="preserve">p t  p              </v>
+        <v xml:space="preserve">p t   p             </v>
       </c>
       <c r="AB1" t="str">
         <f>"'"&amp;AA1&amp;"',"</f>
-        <v>'p t  p              ',</v>
+        <v>'p t   p             ',</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
@@ -61436,7 +61369,7 @@
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>201</v>
+        <v>6</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>6</v>
@@ -61451,7 +61384,7 @@
         <v>6</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>201</v>
+        <v>6</v>
       </c>
       <c r="G6" s="12" t="s">
         <v>6</v>
@@ -61506,16 +61439,16 @@
       </c>
       <c r="AA6" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">p    p              </v>
+        <v xml:space="preserve">                    </v>
       </c>
       <c r="AB6" t="str">
         <f t="shared" si="1"/>
-        <v>'p    p              ',</v>
+        <v>'                    ',</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>6</v>
+        <v>201</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>6</v>
@@ -61533,7 +61466,7 @@
         <v>6</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>6</v>
+        <v>201</v>
       </c>
       <c r="H7" s="12" t="s">
         <v>6</v>
@@ -61585,11 +61518,11 @@
       </c>
       <c r="AA7" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">                    </v>
+        <v xml:space="preserve">p     p             </v>
       </c>
       <c r="AB7" t="str">
         <f t="shared" si="1"/>
-        <v>'                    ',</v>
+        <v>'p     p             ',</v>
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
@@ -62862,12 +62795,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="77" priority="2">
+    <cfRule type="expression" dxfId="88" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="76" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added textured tiles Added basic AI for players
</commit_message>
<xml_diff>
--- a/model/Squoids_data/Squoids floor builder 20180107.xlsx
+++ b/model/Squoids_data/Squoids floor builder 20180107.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7770" windowHeight="540" tabRatio="904" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7770" windowHeight="540" tabRatio="904" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Reverser" sheetId="33" r:id="rId1"/>
@@ -2274,1113 +2274,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="259">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="161">
     <dxf>
       <fill>
         <patternFill>
@@ -4091,6 +2985,426 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -6871,12 +6185,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y26">
-    <cfRule type="expression" dxfId="258" priority="2">
+    <cfRule type="expression" dxfId="160" priority="2">
       <formula>AND(COLUMN()&lt;=$B$27,ROW()&lt;=$B$28)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z26">
-    <cfRule type="cellIs" dxfId="257" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="159" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8724,25 +8038,25 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y5 A6:D8 H6:Y8 A9:Y25">
-    <cfRule type="expression" dxfId="220" priority="5">
+    <cfRule type="expression" dxfId="62" priority="5">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z5 A6:D8 H6:Z8 A9:Z25">
-    <cfRule type="cellIs" dxfId="219" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="4" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA2:AA20">
-    <cfRule type="uniqueValues" dxfId="218" priority="3"/>
+    <cfRule type="uniqueValues" dxfId="60" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6:G8">
-    <cfRule type="expression" dxfId="217" priority="2">
+    <cfRule type="expression" dxfId="59" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6:G8">
-    <cfRule type="cellIs" dxfId="216" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10590,12 +9904,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="215" priority="2">
+    <cfRule type="expression" dxfId="57" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="214" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12443,12 +11757,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="213" priority="2">
+    <cfRule type="expression" dxfId="55" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="212" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14296,12 +13610,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="211" priority="2">
+    <cfRule type="expression" dxfId="53" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="210" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16149,12 +15463,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="209" priority="2">
+    <cfRule type="expression" dxfId="51" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="208" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18005,12 +17319,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="207" priority="2">
+    <cfRule type="expression" dxfId="49" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="206" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19738,22 +19052,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A21:Y25 U1:Y20">
-    <cfRule type="expression" dxfId="205" priority="4">
+    <cfRule type="expression" dxfId="47" priority="4">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:Z25 U1:Z20">
-    <cfRule type="cellIs" dxfId="204" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="3" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:T20">
-    <cfRule type="expression" dxfId="203" priority="2">
+    <cfRule type="expression" dxfId="45" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:T20">
-    <cfRule type="cellIs" dxfId="202" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21479,22 +20793,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A21:Y25 U1:Y20 A19">
-    <cfRule type="expression" dxfId="201" priority="4">
+    <cfRule type="expression" dxfId="43" priority="4">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:Z25 U1:Z20 A19">
-    <cfRule type="cellIs" dxfId="200" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="3" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20 A1:T2 A3:A18 B3:T20">
-    <cfRule type="expression" dxfId="199" priority="2">
+    <cfRule type="expression" dxfId="41" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20 A1:T2 A3:A18 B3:T20">
-    <cfRule type="cellIs" dxfId="198" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23226,22 +22540,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A21:Y25 U1:Y20">
-    <cfRule type="expression" dxfId="197" priority="4">
+    <cfRule type="expression" dxfId="39" priority="4">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:Z25 U1:Z20">
-    <cfRule type="cellIs" dxfId="196" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="3" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:T20">
-    <cfRule type="expression" dxfId="195" priority="2">
+    <cfRule type="expression" dxfId="37" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:T20">
-    <cfRule type="cellIs" dxfId="194" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -24969,22 +24283,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A21:Y25 U1:Y20">
-    <cfRule type="expression" dxfId="193" priority="4">
+    <cfRule type="expression" dxfId="35" priority="4">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:Z25 U1:Z20">
-    <cfRule type="cellIs" dxfId="192" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="3" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:T20">
-    <cfRule type="expression" dxfId="191" priority="2">
+    <cfRule type="expression" dxfId="33" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:T20">
-    <cfRule type="cellIs" dxfId="190" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -26832,12 +26146,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="256" priority="2">
+    <cfRule type="expression" dxfId="158" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="255" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="157" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -28565,22 +27879,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A21:Y25 U1:Y20">
-    <cfRule type="expression" dxfId="189" priority="4">
+    <cfRule type="expression" dxfId="31" priority="4">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:Z25 U1:Z20">
-    <cfRule type="cellIs" dxfId="188" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="3" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:T20">
-    <cfRule type="expression" dxfId="187" priority="2">
+    <cfRule type="expression" dxfId="29" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:T20">
-    <cfRule type="cellIs" dxfId="186" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -30308,12 +29622,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="185" priority="2">
+    <cfRule type="expression" dxfId="27" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="184" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -32041,12 +31355,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="183" priority="2">
+    <cfRule type="expression" dxfId="25" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="182" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -33774,12 +33088,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="181" priority="2">
+    <cfRule type="expression" dxfId="23" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="180" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -35507,22 +34821,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A21:Y25 U1:Y20">
-    <cfRule type="expression" dxfId="179" priority="4">
+    <cfRule type="expression" dxfId="21" priority="4">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:Z25 U1:Z20">
-    <cfRule type="cellIs" dxfId="178" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="3" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:T20">
-    <cfRule type="expression" dxfId="177" priority="2">
+    <cfRule type="expression" dxfId="19" priority="2">
       <formula>AND(COLUMN()&lt;=$B$27,ROW()&lt;=$B$28)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:T20">
-    <cfRule type="cellIs" dxfId="176" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -37250,12 +36564,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="175" priority="2">
+    <cfRule type="expression" dxfId="17" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="174" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -38983,12 +38297,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="173" priority="2">
+    <cfRule type="expression" dxfId="15" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="172" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -40714,12 +40028,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="171" priority="2">
+    <cfRule type="expression" dxfId="13" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="170" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -42567,12 +41881,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="169" priority="2">
+    <cfRule type="expression" dxfId="11" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="168" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -44420,12 +43734,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="167" priority="2">
+    <cfRule type="expression" dxfId="9" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="166" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -46273,12 +45587,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="254" priority="2">
+    <cfRule type="expression" dxfId="156" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="253" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="155" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -48126,12 +47440,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="165" priority="2">
+    <cfRule type="expression" dxfId="7" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="164" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -49979,12 +49293,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="163" priority="2">
+    <cfRule type="expression" dxfId="5" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="162" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -52398,22 +51712,22 @@
     <sortCondition ref="B2:B67"/>
   </sortState>
   <conditionalFormatting sqref="D1:D31 D33:D1048576">
-    <cfRule type="cellIs" dxfId="161" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K31 K33:K77">
-    <cfRule type="cellIs" dxfId="160" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32">
-    <cfRule type="cellIs" dxfId="159" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32">
-    <cfRule type="cellIs" dxfId="158" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -52426,8 +51740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AA20" sqref="AA1:AA20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -52537,7 +51851,7 @@
         <v>6</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>61</v>
+        <v>255</v>
       </c>
       <c r="H2" s="12" t="s">
         <v>6</v>
@@ -52589,11 +51903,11 @@
       </c>
       <c r="AA2" t="str">
         <f t="shared" ref="AA2:AA25" si="0">CONCATENATE(A2,B2,C2,D2,E2,F2,G2,H2,I2,J2,K2,L2,M2,N2,O2,P2,Q2,R2,S2,T2,U2,V2,W2,X2,Y2)</f>
-        <v xml:space="preserve">      *          *  </v>
+        <v xml:space="preserve">      #          *  </v>
       </c>
       <c r="AB2" t="str">
         <f t="shared" ref="AB2:AB20" si="1">"'"&amp;AA2&amp;"',"</f>
-        <v>'      *          *  ',</v>
+        <v>'      #          *  ',</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
@@ -52616,7 +51930,7 @@
         <v>6</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>61</v>
+        <v>255</v>
       </c>
       <c r="H3" s="12" t="s">
         <v>6</v>
@@ -52668,11 +51982,11 @@
       </c>
       <c r="AA3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">*     *     *    *  </v>
+        <v xml:space="preserve">*     #     *    *  </v>
       </c>
       <c r="AB3" t="str">
         <f t="shared" si="1"/>
-        <v>'*     *     *    *  ',</v>
+        <v>'*     #     *    *  ',</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
@@ -52695,7 +52009,7 @@
         <v>6</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>61</v>
+        <v>255</v>
       </c>
       <c r="H4" s="12" t="s">
         <v>6</v>
@@ -52747,11 +52061,11 @@
       </c>
       <c r="AA4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">*     *     *    *  </v>
+        <v xml:space="preserve">*     #     *    *  </v>
       </c>
       <c r="AB4" t="str">
         <f t="shared" si="1"/>
-        <v>'*     *     *    *  ',</v>
+        <v>'*     #     *    *  ',</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
@@ -52774,7 +52088,7 @@
         <v>6</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>61</v>
+        <v>255</v>
       </c>
       <c r="H5" s="12" t="s">
         <v>6</v>
@@ -52826,11 +52140,11 @@
       </c>
       <c r="AA5" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">*     *     *    *  </v>
+        <v xml:space="preserve">*     #     *    *  </v>
       </c>
       <c r="AB5" t="str">
         <f t="shared" si="1"/>
-        <v>'*     *     *    *  ',</v>
+        <v>'*     #     *    *  ',</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
@@ -52853,7 +52167,7 @@
         <v>6</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>61</v>
+        <v>255</v>
       </c>
       <c r="H6" s="12" t="s">
         <v>30</v>
@@ -52905,11 +52219,11 @@
       </c>
       <c r="AA6" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">*     *w    *    *  </v>
+        <v xml:space="preserve">*     #w    *    *  </v>
       </c>
       <c r="AB6" t="str">
         <f t="shared" si="1"/>
-        <v>'*     *w    *    *  ',</v>
+        <v>'*     #w    *    *  ',</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
@@ -52917,19 +52231,19 @@
         <v>264</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>61</v>
+        <v>255</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>61</v>
+        <v>255</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>61</v>
+        <v>255</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>61</v>
+        <v>255</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>61</v>
+        <v>255</v>
       </c>
       <c r="G7" s="12" t="s">
         <v>264</v>
@@ -52984,11 +52298,11 @@
       </c>
       <c r="AA7" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">H*****H     H****H  </v>
+        <v xml:space="preserve">H#####H     H****H  </v>
       </c>
       <c r="AB7" t="str">
         <f t="shared" si="1"/>
-        <v>'H*****H     H****H  ',</v>
+        <v>'H#####H     H****H  ',</v>
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
@@ -53041,7 +52355,7 @@
         <v>6</v>
       </c>
       <c r="Q8" s="12" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="R8" s="12" t="s">
         <v>6</v>
@@ -53063,11 +52377,11 @@
       </c>
       <c r="AA8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">     w              </v>
+        <v xml:space="preserve">     w          w   </v>
       </c>
       <c r="AB8" t="str">
         <f t="shared" si="1"/>
-        <v>'     w              ',</v>
+        <v>'     w          w   ',</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
@@ -53199,7 +52513,7 @@
         <v>6</v>
       </c>
       <c r="Q10" s="12" t="s">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="R10" s="12" t="s">
         <v>6</v>
@@ -53221,11 +52535,11 @@
       </c>
       <c r="AA10" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">                w   </v>
+        <v xml:space="preserve">                    </v>
       </c>
       <c r="AB10" t="str">
         <f t="shared" si="1"/>
-        <v>'                w   ',</v>
+        <v>'                    ',</v>
       </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
@@ -54258,12 +53572,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="252" priority="2">
+    <cfRule type="expression" dxfId="154" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="251" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="153" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -56111,82 +55425,82 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A21:Y25 G1:N6 G6:G7 S1:Y6 M5:N7 L12:Q17 G16:Y20 A18:F20 I15:Y15 A7:Y14">
-    <cfRule type="expression" dxfId="250" priority="16">
+    <cfRule type="expression" dxfId="152" priority="16">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:Z25 G1:N6 G6:G7 S1:Z6 M5:N7 L12:Q17 G16:Z20 A18:F20 I15:Z15 A7:Z14">
-    <cfRule type="cellIs" dxfId="249" priority="15" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="151" priority="15" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G15:H15 A12:G17">
-    <cfRule type="expression" dxfId="248" priority="14">
+    <cfRule type="expression" dxfId="150" priority="14">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G15:H15 A12:G17">
-    <cfRule type="cellIs" dxfId="247" priority="13" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="149" priority="13" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M1:R7">
-    <cfRule type="expression" dxfId="246" priority="12">
+    <cfRule type="expression" dxfId="148" priority="12">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M1:R7">
-    <cfRule type="cellIs" dxfId="245" priority="11" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="147" priority="11" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:G7">
-    <cfRule type="expression" dxfId="244" priority="10">
+    <cfRule type="expression" dxfId="146" priority="10">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:G7">
-    <cfRule type="cellIs" dxfId="243" priority="9" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="145" priority="9" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15:E15">
-    <cfRule type="expression" dxfId="127" priority="8">
+    <cfRule type="expression" dxfId="144" priority="8">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15:E15">
-    <cfRule type="cellIs" dxfId="125" priority="7" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="7" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:E16">
-    <cfRule type="expression" dxfId="121" priority="6">
+    <cfRule type="expression" dxfId="142" priority="6">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:E16">
-    <cfRule type="cellIs" dxfId="119" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="141" priority="5" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F15">
-    <cfRule type="expression" dxfId="9" priority="4">
+    <cfRule type="expression" dxfId="140" priority="4">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F15">
-    <cfRule type="cellIs" dxfId="7" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="139" priority="3" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F16">
-    <cfRule type="expression" dxfId="5" priority="2">
+    <cfRule type="expression" dxfId="138" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F16">
-    <cfRule type="cellIs" dxfId="3" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -56199,7 +55513,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AA20" sqref="AA1:AA20"/>
     </sheetView>
   </sheetViews>
@@ -58034,62 +57348,62 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="U1:Y6 F1:N5 A6:N6 M1:O7 A7:Y25">
-    <cfRule type="expression" dxfId="242" priority="14">
+    <cfRule type="expression" dxfId="136" priority="14">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1:Z6 F1:N5 A6:N6 M1:O7 A7:Z25">
-    <cfRule type="cellIs" dxfId="241" priority="13" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="135" priority="13" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:E5">
-    <cfRule type="expression" dxfId="240" priority="10">
+    <cfRule type="expression" dxfId="134" priority="10">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:E5">
-    <cfRule type="cellIs" dxfId="239" priority="9" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="133" priority="9" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:T6 M6:R7">
-    <cfRule type="expression" dxfId="238" priority="8">
+    <cfRule type="expression" dxfId="132" priority="8">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:T6 M6:R7">
-    <cfRule type="cellIs" dxfId="237" priority="7" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="7" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F5">
-    <cfRule type="expression" dxfId="157" priority="6">
+    <cfRule type="expression" dxfId="130" priority="6">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F5">
-    <cfRule type="cellIs" dxfId="156" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="129" priority="5" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:E6">
-    <cfRule type="expression" dxfId="155" priority="4">
+    <cfRule type="expression" dxfId="128" priority="4">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:E6">
-    <cfRule type="cellIs" dxfId="154" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="3" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6">
-    <cfRule type="expression" dxfId="153" priority="2">
+    <cfRule type="expression" dxfId="126" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6">
-    <cfRule type="cellIs" dxfId="152" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -59937,292 +59251,292 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A8:Y25 G1:N1 S1:Y7 A7:N7 F2:N5 B6:N6">
-    <cfRule type="expression" dxfId="236" priority="58">
+    <cfRule type="expression" dxfId="124" priority="58">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8:Z25 G1:N1 S1:Z7 A7:N7 F2:N5 B6:N6">
-    <cfRule type="cellIs" dxfId="235" priority="57" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="57" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:E5">
-    <cfRule type="expression" dxfId="234" priority="56">
+    <cfRule type="expression" dxfId="122" priority="56">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:E5">
-    <cfRule type="cellIs" dxfId="233" priority="55" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="121" priority="55" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M1:R7">
-    <cfRule type="expression" dxfId="232" priority="54">
+    <cfRule type="expression" dxfId="120" priority="54">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M1:R7">
-    <cfRule type="cellIs" dxfId="231" priority="53" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="53" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6">
-    <cfRule type="expression" dxfId="230" priority="52">
+    <cfRule type="expression" dxfId="118" priority="52">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6">
-    <cfRule type="cellIs" dxfId="229" priority="51" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="51" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1">
-    <cfRule type="expression" dxfId="228" priority="50">
+    <cfRule type="expression" dxfId="116" priority="50">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1">
-    <cfRule type="cellIs" dxfId="227" priority="49" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="49" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6">
-    <cfRule type="expression" dxfId="226" priority="48">
+    <cfRule type="expression" dxfId="114" priority="48">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6">
-    <cfRule type="cellIs" dxfId="225" priority="47" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="47" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F5">
-    <cfRule type="expression" dxfId="151" priority="46">
+    <cfRule type="expression" dxfId="112" priority="46">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F5">
-    <cfRule type="cellIs" dxfId="150" priority="45" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="45" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1">
-    <cfRule type="expression" dxfId="149" priority="44">
+    <cfRule type="expression" dxfId="110" priority="44">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1">
-    <cfRule type="cellIs" dxfId="148" priority="43" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="43" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6">
-    <cfRule type="expression" dxfId="147" priority="42">
+    <cfRule type="expression" dxfId="108" priority="42">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6">
-    <cfRule type="cellIs" dxfId="146" priority="41" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="41" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:E6">
-    <cfRule type="expression" dxfId="145" priority="40">
+    <cfRule type="expression" dxfId="106" priority="40">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:E6">
-    <cfRule type="cellIs" dxfId="144" priority="39" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="39" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7">
-    <cfRule type="expression" dxfId="143" priority="38">
+    <cfRule type="expression" dxfId="104" priority="38">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7">
-    <cfRule type="cellIs" dxfId="142" priority="37" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="37" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7">
-    <cfRule type="expression" dxfId="141" priority="36">
+    <cfRule type="expression" dxfId="102" priority="36">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7">
-    <cfRule type="cellIs" dxfId="140" priority="35" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="35" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6">
-    <cfRule type="expression" dxfId="139" priority="34">
+    <cfRule type="expression" dxfId="100" priority="34">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6">
-    <cfRule type="cellIs" dxfId="138" priority="33" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="33" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7">
-    <cfRule type="expression" dxfId="137" priority="32">
+    <cfRule type="expression" dxfId="98" priority="32">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7">
-    <cfRule type="cellIs" dxfId="136" priority="31" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="31" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2">
-    <cfRule type="expression" dxfId="107" priority="30">
+    <cfRule type="expression" dxfId="96" priority="30">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2">
-    <cfRule type="cellIs" dxfId="105" priority="29" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="29" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P2">
-    <cfRule type="expression" dxfId="101" priority="28">
+    <cfRule type="expression" dxfId="94" priority="28">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P2">
-    <cfRule type="cellIs" dxfId="99" priority="27" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="27" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2">
-    <cfRule type="expression" dxfId="95" priority="26">
+    <cfRule type="expression" dxfId="92" priority="26">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2">
-    <cfRule type="cellIs" dxfId="93" priority="25" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="25" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O3">
-    <cfRule type="expression" dxfId="85" priority="24">
+    <cfRule type="expression" dxfId="90" priority="24">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O3">
-    <cfRule type="cellIs" dxfId="83" priority="23" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="23" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P3">
-    <cfRule type="expression" dxfId="81" priority="22">
+    <cfRule type="expression" dxfId="88" priority="22">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P3">
-    <cfRule type="cellIs" dxfId="79" priority="21" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="21" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q3">
-    <cfRule type="expression" dxfId="77" priority="20">
+    <cfRule type="expression" dxfId="86" priority="20">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q3">
-    <cfRule type="cellIs" dxfId="75" priority="19" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="19" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O4">
-    <cfRule type="expression" dxfId="69" priority="18">
+    <cfRule type="expression" dxfId="84" priority="18">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O4">
-    <cfRule type="cellIs" dxfId="67" priority="17" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="17" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4">
-    <cfRule type="expression" dxfId="65" priority="16">
+    <cfRule type="expression" dxfId="82" priority="16">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4">
-    <cfRule type="cellIs" dxfId="63" priority="15" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="15" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q4">
-    <cfRule type="expression" dxfId="61" priority="14">
+    <cfRule type="expression" dxfId="80" priority="14">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q4">
-    <cfRule type="cellIs" dxfId="59" priority="13" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="13" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O5">
-    <cfRule type="expression" dxfId="53" priority="12">
+    <cfRule type="expression" dxfId="78" priority="12">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O5">
-    <cfRule type="cellIs" dxfId="51" priority="11" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="11" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P5">
-    <cfRule type="expression" dxfId="49" priority="10">
+    <cfRule type="expression" dxfId="76" priority="10">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P5">
-    <cfRule type="cellIs" dxfId="47" priority="9" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="9" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q5">
-    <cfRule type="expression" dxfId="45" priority="8">
+    <cfRule type="expression" dxfId="74" priority="8">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q5">
-    <cfRule type="cellIs" dxfId="43" priority="7" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="7" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O6">
-    <cfRule type="expression" dxfId="37" priority="6">
+    <cfRule type="expression" dxfId="72" priority="6">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O6">
-    <cfRule type="cellIs" dxfId="35" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="5" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P6">
-    <cfRule type="expression" dxfId="33" priority="4">
+    <cfRule type="expression" dxfId="70" priority="4">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P6">
-    <cfRule type="cellIs" dxfId="31" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="3" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q6">
-    <cfRule type="expression" dxfId="29" priority="2">
+    <cfRule type="expression" dxfId="68" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q6">
-    <cfRule type="cellIs" dxfId="27" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -60346,7 +59660,7 @@
         <v>285</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>61</v>
+        <v>255</v>
       </c>
       <c r="H2" s="12" t="s">
         <v>6</v>
@@ -60398,11 +59712,11 @@
       </c>
       <c r="AA2" t="str">
         <f t="shared" ref="AA2:AA25" si="0">CONCATENATE(A2,B2,C2,D2,E2,F2,G2,H2,I2,J2,K2,L2,M2,N2,O2,P2,Q2,R2,S2,T2,U2,V2,W2,X2,Y2)</f>
-        <v xml:space="preserve">*@@@@@*         T   </v>
+        <v xml:space="preserve">*@@@@@#         T   </v>
       </c>
       <c r="AB2" t="str">
         <f t="shared" ref="AB2:AB20" si="1">"'"&amp;AA2&amp;"',"</f>
-        <v>'*@@@@@*         T   ',</v>
+        <v>'*@@@@@#         T   ',</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
@@ -60425,7 +59739,7 @@
         <v>285</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>61</v>
+        <v>255</v>
       </c>
       <c r="H3" s="12" t="s">
         <v>6</v>
@@ -60477,11 +59791,11 @@
       </c>
       <c r="AA3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">*@@@@@*             </v>
+        <v xml:space="preserve">*@@@@@#             </v>
       </c>
       <c r="AB3" t="str">
         <f t="shared" si="1"/>
-        <v>'*@@@@@*             ',</v>
+        <v>'*@@@@@#             ',</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
@@ -60504,7 +59818,7 @@
         <v>285</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>61</v>
+        <v>255</v>
       </c>
       <c r="H4" s="12" t="s">
         <v>6</v>
@@ -60556,11 +59870,11 @@
       </c>
       <c r="AA4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">*@@@@@*             </v>
+        <v xml:space="preserve">*@@@@@#             </v>
       </c>
       <c r="AB4" t="str">
         <f t="shared" si="1"/>
-        <v>'*@@@@@*             ',</v>
+        <v>'*@@@@@#             ',</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
@@ -60583,7 +59897,7 @@
         <v>285</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>61</v>
+        <v>255</v>
       </c>
       <c r="H5" s="12" t="s">
         <v>6</v>
@@ -60635,11 +59949,11 @@
       </c>
       <c r="AA5" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">*@@@@@*             </v>
+        <v xml:space="preserve">*@@@@@#             </v>
       </c>
       <c r="AB5" t="str">
         <f t="shared" si="1"/>
-        <v>'*@@@@@*             ',</v>
+        <v>'*@@@@@#             ',</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
@@ -60662,7 +59976,7 @@
         <v>285</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>61</v>
+        <v>255</v>
       </c>
       <c r="H6" s="12" t="s">
         <v>6</v>
@@ -60714,11 +60028,11 @@
       </c>
       <c r="AA6" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">*@@@@@*      t      </v>
+        <v xml:space="preserve">*@@@@@#      t      </v>
       </c>
       <c r="AB6" t="str">
         <f t="shared" si="1"/>
-        <v>'*@@@@@*      t      ',</v>
+        <v>'*@@@@@#      t      ',</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
@@ -60726,19 +60040,19 @@
         <v>264</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>61</v>
+        <v>255</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>61</v>
+        <v>255</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>61</v>
+        <v>255</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>61</v>
+        <v>255</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>61</v>
+        <v>255</v>
       </c>
       <c r="G7" s="12" t="s">
         <v>264</v>
@@ -60793,11 +60107,11 @@
       </c>
       <c r="AA7" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">H*****H     p    p  </v>
+        <v xml:space="preserve">H#####H     p    p  </v>
       </c>
       <c r="AB7" t="str">
         <f t="shared" si="1"/>
-        <v>'H*****H     p    p  ',</v>
+        <v>'H#####H     p    p  ',</v>
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
@@ -62070,12 +61384,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="224" priority="2">
+    <cfRule type="expression" dxfId="66" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="223" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -63923,12 +63237,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="222" priority="2">
+    <cfRule type="expression" dxfId="64" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="221" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>